<commit_message>
Fixed SAFE-OP errors, adopted and modified original SPI API
</commit_message>
<xml_diff>
--- a/ESC_Folder/TENCL040_ESC.xlsx
+++ b/ESC_Folder/TENCL040_ESC.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t xml:space="preserve">Device Profile:</t>
   </si>
@@ -340,6 +340,18 @@
   </si>
   <si>
     <t xml:space="preserve">ro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x6008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UINT16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tx</t>
   </si>
   <si>
     <t xml:space="preserve">//0x7nnx</t>
@@ -646,10 +658,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -659,6 +667,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -885,9 +897,9 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="10" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="10" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F196" activeCellId="0" sqref="F196"/>
+      <selection pane="bottomLeft" activeCell="N171" activeCellId="0" sqref="N171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -2589,7 +2601,7 @@
       <c r="P153" s="34"/>
       <c r="Q153" s="34"/>
     </row>
-    <row r="154" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="23"/>
       <c r="B154" s="22"/>
       <c r="C154" s="23"/>
@@ -2607,6 +2619,1013 @@
       <c r="O154" s="34"/>
       <c r="P154" s="34"/>
       <c r="Q154" s="34"/>
+      <c r="R154" s="15"/>
+      <c r="S154" s="15"/>
+      <c r="T154" s="15"/>
+      <c r="U154" s="15"/>
+      <c r="V154" s="15"/>
+      <c r="W154" s="15"/>
+      <c r="X154" s="15"/>
+      <c r="Y154" s="15"/>
+      <c r="Z154" s="15"/>
+      <c r="AA154" s="15"/>
+      <c r="AB154" s="15"/>
+      <c r="AC154" s="15"/>
+      <c r="AD154" s="15"/>
+      <c r="AE154" s="15"/>
+      <c r="AF154" s="15"/>
+      <c r="AG154" s="15"/>
+      <c r="AH154" s="15"/>
+      <c r="AI154" s="15"/>
+      <c r="AJ154" s="15"/>
+      <c r="AK154" s="15"/>
+      <c r="AL154" s="15"/>
+      <c r="AM154" s="15"/>
+      <c r="AN154" s="15"/>
+      <c r="AO154" s="15"/>
+      <c r="AP154" s="15"/>
+      <c r="AQ154" s="15"/>
+      <c r="AR154" s="15"/>
+      <c r="AS154" s="15"/>
+      <c r="AT154" s="15"/>
+      <c r="AU154" s="15"/>
+      <c r="AV154" s="15"/>
+      <c r="AW154" s="15"/>
+      <c r="AX154" s="15"/>
+      <c r="AY154" s="15"/>
+      <c r="AZ154" s="15"/>
+      <c r="BA154" s="15"/>
+      <c r="BB154" s="15"/>
+      <c r="BC154" s="15"/>
+      <c r="BD154" s="15"/>
+      <c r="BE154" s="15"/>
+      <c r="BF154" s="15"/>
+      <c r="BG154" s="15"/>
+      <c r="BH154" s="15"/>
+      <c r="BI154" s="15"/>
+      <c r="BJ154" s="15"/>
+      <c r="BK154" s="15"/>
+      <c r="BL154" s="15"/>
+      <c r="BM154" s="15"/>
+      <c r="BN154" s="15"/>
+      <c r="BO154" s="15"/>
+      <c r="BP154" s="15"/>
+      <c r="BQ154" s="15"/>
+      <c r="BR154" s="15"/>
+      <c r="BS154" s="15"/>
+      <c r="BT154" s="15"/>
+      <c r="BU154" s="15"/>
+      <c r="BV154" s="15"/>
+      <c r="BW154" s="15"/>
+      <c r="BX154" s="15"/>
+      <c r="BY154" s="15"/>
+      <c r="BZ154" s="15"/>
+      <c r="CA154" s="15"/>
+      <c r="CB154" s="15"/>
+      <c r="CC154" s="15"/>
+      <c r="CD154" s="15"/>
+      <c r="CE154" s="15"/>
+      <c r="CF154" s="15"/>
+      <c r="CG154" s="15"/>
+      <c r="CH154" s="15"/>
+      <c r="CI154" s="15"/>
+      <c r="CJ154" s="15"/>
+      <c r="CK154" s="15"/>
+      <c r="CL154" s="15"/>
+      <c r="CM154" s="15"/>
+      <c r="CN154" s="15"/>
+      <c r="CO154" s="15"/>
+      <c r="CP154" s="15"/>
+      <c r="CQ154" s="15"/>
+      <c r="CR154" s="15"/>
+      <c r="CS154" s="15"/>
+      <c r="CT154" s="15"/>
+      <c r="CU154" s="15"/>
+      <c r="CV154" s="15"/>
+      <c r="CW154" s="15"/>
+      <c r="CX154" s="15"/>
+      <c r="CY154" s="15"/>
+      <c r="CZ154" s="15"/>
+      <c r="DA154" s="15"/>
+      <c r="DB154" s="15"/>
+      <c r="DC154" s="15"/>
+      <c r="DD154" s="15"/>
+      <c r="DE154" s="15"/>
+      <c r="DF154" s="15"/>
+      <c r="DG154" s="15"/>
+      <c r="DH154" s="15"/>
+      <c r="DI154" s="15"/>
+      <c r="DJ154" s="15"/>
+      <c r="DK154" s="15"/>
+      <c r="DL154" s="15"/>
+      <c r="DM154" s="15"/>
+      <c r="DN154" s="15"/>
+      <c r="DO154" s="15"/>
+      <c r="DP154" s="15"/>
+      <c r="DQ154" s="15"/>
+      <c r="DR154" s="15"/>
+      <c r="DS154" s="15"/>
+      <c r="DT154" s="15"/>
+      <c r="DU154" s="15"/>
+      <c r="DV154" s="15"/>
+      <c r="DW154" s="15"/>
+      <c r="DX154" s="15"/>
+      <c r="DY154" s="15"/>
+      <c r="DZ154" s="15"/>
+      <c r="EA154" s="15"/>
+      <c r="EB154" s="15"/>
+      <c r="EC154" s="15"/>
+      <c r="ED154" s="15"/>
+      <c r="EE154" s="15"/>
+      <c r="EF154" s="15"/>
+      <c r="EG154" s="15"/>
+      <c r="EH154" s="15"/>
+      <c r="EI154" s="15"/>
+      <c r="EJ154" s="15"/>
+      <c r="EK154" s="15"/>
+      <c r="EL154" s="15"/>
+      <c r="EM154" s="15"/>
+      <c r="EN154" s="15"/>
+      <c r="EO154" s="15"/>
+      <c r="EP154" s="15"/>
+      <c r="EQ154" s="15"/>
+      <c r="ER154" s="15"/>
+      <c r="ES154" s="15"/>
+      <c r="ET154" s="15"/>
+      <c r="EU154" s="15"/>
+      <c r="EV154" s="15"/>
+      <c r="EW154" s="15"/>
+      <c r="EX154" s="15"/>
+      <c r="EY154" s="15"/>
+      <c r="EZ154" s="15"/>
+      <c r="FA154" s="15"/>
+      <c r="FB154" s="15"/>
+      <c r="FC154" s="15"/>
+      <c r="FD154" s="15"/>
+      <c r="FE154" s="15"/>
+      <c r="FF154" s="15"/>
+      <c r="FG154" s="15"/>
+      <c r="FH154" s="15"/>
+      <c r="FI154" s="15"/>
+      <c r="FJ154" s="15"/>
+      <c r="FK154" s="15"/>
+      <c r="FL154" s="15"/>
+      <c r="FM154" s="15"/>
+      <c r="FN154" s="15"/>
+      <c r="FO154" s="15"/>
+      <c r="FP154" s="15"/>
+      <c r="FQ154" s="15"/>
+      <c r="FR154" s="15"/>
+      <c r="FS154" s="15"/>
+      <c r="FT154" s="15"/>
+      <c r="FU154" s="15"/>
+      <c r="FV154" s="15"/>
+      <c r="FW154" s="15"/>
+      <c r="FX154" s="15"/>
+      <c r="FY154" s="15"/>
+      <c r="FZ154" s="15"/>
+      <c r="GA154" s="15"/>
+      <c r="GB154" s="15"/>
+      <c r="GC154" s="15"/>
+      <c r="GD154" s="15"/>
+      <c r="GE154" s="15"/>
+      <c r="GF154" s="15"/>
+      <c r="GG154" s="15"/>
+      <c r="GH154" s="15"/>
+      <c r="GI154" s="15"/>
+      <c r="GJ154" s="15"/>
+      <c r="GK154" s="15"/>
+      <c r="GL154" s="15"/>
+      <c r="GM154" s="15"/>
+      <c r="GN154" s="15"/>
+      <c r="GO154" s="15"/>
+      <c r="GP154" s="15"/>
+      <c r="GQ154" s="15"/>
+      <c r="GR154" s="15"/>
+      <c r="GS154" s="15"/>
+      <c r="GT154" s="15"/>
+      <c r="GU154" s="15"/>
+      <c r="GV154" s="15"/>
+      <c r="GW154" s="15"/>
+      <c r="GX154" s="15"/>
+      <c r="GY154" s="15"/>
+      <c r="GZ154" s="15"/>
+      <c r="HA154" s="15"/>
+      <c r="HB154" s="15"/>
+      <c r="HC154" s="15"/>
+      <c r="HD154" s="15"/>
+      <c r="HE154" s="15"/>
+      <c r="HF154" s="15"/>
+      <c r="HG154" s="15"/>
+      <c r="HH154" s="15"/>
+      <c r="HI154" s="15"/>
+      <c r="HJ154" s="15"/>
+      <c r="HK154" s="15"/>
+      <c r="HL154" s="15"/>
+      <c r="HM154" s="15"/>
+      <c r="HN154" s="15"/>
+      <c r="HO154" s="15"/>
+      <c r="HP154" s="15"/>
+      <c r="HQ154" s="15"/>
+      <c r="HR154" s="15"/>
+      <c r="HS154" s="15"/>
+      <c r="HT154" s="15"/>
+      <c r="HU154" s="15"/>
+      <c r="HV154" s="15"/>
+      <c r="HW154" s="15"/>
+      <c r="HX154" s="15"/>
+      <c r="HY154" s="15"/>
+      <c r="HZ154" s="15"/>
+      <c r="IA154" s="15"/>
+      <c r="IB154" s="15"/>
+      <c r="IC154" s="15"/>
+      <c r="ID154" s="15"/>
+      <c r="IE154" s="15"/>
+      <c r="IF154" s="15"/>
+      <c r="IG154" s="15"/>
+      <c r="IH154" s="15"/>
+      <c r="II154" s="15"/>
+      <c r="IJ154" s="15"/>
+      <c r="IK154" s="15"/>
+      <c r="IL154" s="15"/>
+      <c r="IM154" s="15"/>
+      <c r="IN154" s="15"/>
+      <c r="IO154" s="15"/>
+      <c r="IP154" s="15"/>
+      <c r="IQ154" s="15"/>
+      <c r="IR154" s="15"/>
+      <c r="IS154" s="15"/>
+      <c r="IT154" s="15"/>
+      <c r="IU154" s="15"/>
+      <c r="IV154" s="15"/>
+      <c r="IW154" s="15"/>
+      <c r="IX154" s="15"/>
+      <c r="IY154" s="15"/>
+      <c r="IZ154" s="15"/>
+      <c r="JA154" s="15"/>
+      <c r="JB154" s="15"/>
+      <c r="JC154" s="15"/>
+      <c r="JD154" s="15"/>
+      <c r="JE154" s="15"/>
+      <c r="JF154" s="15"/>
+      <c r="JG154" s="15"/>
+      <c r="JH154" s="15"/>
+      <c r="JI154" s="15"/>
+      <c r="JJ154" s="15"/>
+      <c r="JK154" s="15"/>
+      <c r="JL154" s="15"/>
+      <c r="JM154" s="15"/>
+      <c r="JN154" s="15"/>
+      <c r="JO154" s="15"/>
+      <c r="JP154" s="15"/>
+      <c r="JQ154" s="15"/>
+      <c r="JR154" s="15"/>
+      <c r="JS154" s="15"/>
+      <c r="JT154" s="15"/>
+      <c r="JU154" s="15"/>
+      <c r="JV154" s="15"/>
+      <c r="JW154" s="15"/>
+      <c r="JX154" s="15"/>
+      <c r="JY154" s="15"/>
+      <c r="JZ154" s="15"/>
+      <c r="KA154" s="15"/>
+      <c r="KB154" s="15"/>
+      <c r="KC154" s="15"/>
+      <c r="KD154" s="15"/>
+      <c r="KE154" s="15"/>
+      <c r="KF154" s="15"/>
+      <c r="KG154" s="15"/>
+      <c r="KH154" s="15"/>
+      <c r="KI154" s="15"/>
+      <c r="KJ154" s="15"/>
+      <c r="KK154" s="15"/>
+      <c r="KL154" s="15"/>
+      <c r="KM154" s="15"/>
+      <c r="KN154" s="15"/>
+      <c r="KO154" s="15"/>
+      <c r="KP154" s="15"/>
+      <c r="KQ154" s="15"/>
+      <c r="KR154" s="15"/>
+      <c r="KS154" s="15"/>
+      <c r="KT154" s="15"/>
+      <c r="KU154" s="15"/>
+      <c r="KV154" s="15"/>
+      <c r="KW154" s="15"/>
+      <c r="KX154" s="15"/>
+      <c r="KY154" s="15"/>
+      <c r="KZ154" s="15"/>
+      <c r="LA154" s="15"/>
+      <c r="LB154" s="15"/>
+      <c r="LC154" s="15"/>
+      <c r="LD154" s="15"/>
+      <c r="LE154" s="15"/>
+      <c r="LF154" s="15"/>
+      <c r="LG154" s="15"/>
+      <c r="LH154" s="15"/>
+      <c r="LI154" s="15"/>
+      <c r="LJ154" s="15"/>
+      <c r="LK154" s="15"/>
+      <c r="LL154" s="15"/>
+      <c r="LM154" s="15"/>
+      <c r="LN154" s="15"/>
+      <c r="LO154" s="15"/>
+      <c r="LP154" s="15"/>
+      <c r="LQ154" s="15"/>
+      <c r="LR154" s="15"/>
+      <c r="LS154" s="15"/>
+      <c r="LT154" s="15"/>
+      <c r="LU154" s="15"/>
+      <c r="LV154" s="15"/>
+      <c r="LW154" s="15"/>
+      <c r="LX154" s="15"/>
+      <c r="LY154" s="15"/>
+      <c r="LZ154" s="15"/>
+      <c r="MA154" s="15"/>
+      <c r="MB154" s="15"/>
+      <c r="MC154" s="15"/>
+      <c r="MD154" s="15"/>
+      <c r="ME154" s="15"/>
+      <c r="MF154" s="15"/>
+      <c r="MG154" s="15"/>
+      <c r="MH154" s="15"/>
+      <c r="MI154" s="15"/>
+      <c r="MJ154" s="15"/>
+      <c r="MK154" s="15"/>
+      <c r="ML154" s="15"/>
+      <c r="MM154" s="15"/>
+      <c r="MN154" s="15"/>
+      <c r="MO154" s="15"/>
+      <c r="MP154" s="15"/>
+      <c r="MQ154" s="15"/>
+      <c r="MR154" s="15"/>
+      <c r="MS154" s="15"/>
+      <c r="MT154" s="15"/>
+      <c r="MU154" s="15"/>
+      <c r="MV154" s="15"/>
+      <c r="MW154" s="15"/>
+      <c r="MX154" s="15"/>
+      <c r="MY154" s="15"/>
+      <c r="MZ154" s="15"/>
+      <c r="NA154" s="15"/>
+      <c r="NB154" s="15"/>
+      <c r="NC154" s="15"/>
+      <c r="ND154" s="15"/>
+      <c r="NE154" s="15"/>
+      <c r="NF154" s="15"/>
+      <c r="NG154" s="15"/>
+      <c r="NH154" s="15"/>
+      <c r="NI154" s="15"/>
+      <c r="NJ154" s="15"/>
+      <c r="NK154" s="15"/>
+      <c r="NL154" s="15"/>
+      <c r="NM154" s="15"/>
+      <c r="NN154" s="15"/>
+      <c r="NO154" s="15"/>
+      <c r="NP154" s="15"/>
+      <c r="NQ154" s="15"/>
+      <c r="NR154" s="15"/>
+      <c r="NS154" s="15"/>
+      <c r="NT154" s="15"/>
+      <c r="NU154" s="15"/>
+      <c r="NV154" s="15"/>
+      <c r="NW154" s="15"/>
+      <c r="NX154" s="15"/>
+      <c r="NY154" s="15"/>
+      <c r="NZ154" s="15"/>
+      <c r="OA154" s="15"/>
+      <c r="OB154" s="15"/>
+      <c r="OC154" s="15"/>
+      <c r="OD154" s="15"/>
+      <c r="OE154" s="15"/>
+      <c r="OF154" s="15"/>
+      <c r="OG154" s="15"/>
+      <c r="OH154" s="15"/>
+      <c r="OI154" s="15"/>
+      <c r="OJ154" s="15"/>
+      <c r="OK154" s="15"/>
+      <c r="OL154" s="15"/>
+      <c r="OM154" s="15"/>
+      <c r="ON154" s="15"/>
+      <c r="OO154" s="15"/>
+      <c r="OP154" s="15"/>
+      <c r="OQ154" s="15"/>
+      <c r="OR154" s="15"/>
+      <c r="OS154" s="15"/>
+      <c r="OT154" s="15"/>
+      <c r="OU154" s="15"/>
+      <c r="OV154" s="15"/>
+      <c r="OW154" s="15"/>
+      <c r="OX154" s="15"/>
+      <c r="OY154" s="15"/>
+      <c r="OZ154" s="15"/>
+      <c r="PA154" s="15"/>
+      <c r="PB154" s="15"/>
+      <c r="PC154" s="15"/>
+      <c r="PD154" s="15"/>
+      <c r="PE154" s="15"/>
+      <c r="PF154" s="15"/>
+      <c r="PG154" s="15"/>
+      <c r="PH154" s="15"/>
+      <c r="PI154" s="15"/>
+      <c r="PJ154" s="15"/>
+      <c r="PK154" s="15"/>
+      <c r="PL154" s="15"/>
+      <c r="PM154" s="15"/>
+      <c r="PN154" s="15"/>
+      <c r="PO154" s="15"/>
+      <c r="PP154" s="15"/>
+      <c r="PQ154" s="15"/>
+      <c r="PR154" s="15"/>
+      <c r="PS154" s="15"/>
+      <c r="PT154" s="15"/>
+      <c r="PU154" s="15"/>
+      <c r="PV154" s="15"/>
+      <c r="PW154" s="15"/>
+      <c r="PX154" s="15"/>
+      <c r="PY154" s="15"/>
+      <c r="PZ154" s="15"/>
+      <c r="QA154" s="15"/>
+      <c r="QB154" s="15"/>
+      <c r="QC154" s="15"/>
+      <c r="QD154" s="15"/>
+      <c r="QE154" s="15"/>
+      <c r="QF154" s="15"/>
+      <c r="QG154" s="15"/>
+      <c r="QH154" s="15"/>
+      <c r="QI154" s="15"/>
+      <c r="QJ154" s="15"/>
+      <c r="QK154" s="15"/>
+      <c r="QL154" s="15"/>
+      <c r="QM154" s="15"/>
+      <c r="QN154" s="15"/>
+      <c r="QO154" s="15"/>
+      <c r="QP154" s="15"/>
+      <c r="QQ154" s="15"/>
+      <c r="QR154" s="15"/>
+      <c r="QS154" s="15"/>
+      <c r="QT154" s="15"/>
+      <c r="QU154" s="15"/>
+      <c r="QV154" s="15"/>
+      <c r="QW154" s="15"/>
+      <c r="QX154" s="15"/>
+      <c r="QY154" s="15"/>
+      <c r="QZ154" s="15"/>
+      <c r="RA154" s="15"/>
+      <c r="RB154" s="15"/>
+      <c r="RC154" s="15"/>
+      <c r="RD154" s="15"/>
+      <c r="RE154" s="15"/>
+      <c r="RF154" s="15"/>
+      <c r="RG154" s="15"/>
+      <c r="RH154" s="15"/>
+      <c r="RI154" s="15"/>
+      <c r="RJ154" s="15"/>
+      <c r="RK154" s="15"/>
+      <c r="RL154" s="15"/>
+      <c r="RM154" s="15"/>
+      <c r="RN154" s="15"/>
+      <c r="RO154" s="15"/>
+      <c r="RP154" s="15"/>
+      <c r="RQ154" s="15"/>
+      <c r="RR154" s="15"/>
+      <c r="RS154" s="15"/>
+      <c r="RT154" s="15"/>
+      <c r="RU154" s="15"/>
+      <c r="RV154" s="15"/>
+      <c r="RW154" s="15"/>
+      <c r="RX154" s="15"/>
+      <c r="RY154" s="15"/>
+      <c r="RZ154" s="15"/>
+      <c r="SA154" s="15"/>
+      <c r="SB154" s="15"/>
+      <c r="SC154" s="15"/>
+      <c r="SD154" s="15"/>
+      <c r="SE154" s="15"/>
+      <c r="SF154" s="15"/>
+      <c r="SG154" s="15"/>
+      <c r="SH154" s="15"/>
+      <c r="SI154" s="15"/>
+      <c r="SJ154" s="15"/>
+      <c r="SK154" s="15"/>
+      <c r="SL154" s="15"/>
+      <c r="SM154" s="15"/>
+      <c r="SN154" s="15"/>
+      <c r="SO154" s="15"/>
+      <c r="SP154" s="15"/>
+      <c r="SQ154" s="15"/>
+      <c r="SR154" s="15"/>
+      <c r="SS154" s="15"/>
+      <c r="ST154" s="15"/>
+      <c r="SU154" s="15"/>
+      <c r="SV154" s="15"/>
+      <c r="SW154" s="15"/>
+      <c r="SX154" s="15"/>
+      <c r="SY154" s="15"/>
+      <c r="SZ154" s="15"/>
+      <c r="TA154" s="15"/>
+      <c r="TB154" s="15"/>
+      <c r="TC154" s="15"/>
+      <c r="TD154" s="15"/>
+      <c r="TE154" s="15"/>
+      <c r="TF154" s="15"/>
+      <c r="TG154" s="15"/>
+      <c r="TH154" s="15"/>
+      <c r="TI154" s="15"/>
+      <c r="TJ154" s="15"/>
+      <c r="TK154" s="15"/>
+      <c r="TL154" s="15"/>
+      <c r="TM154" s="15"/>
+      <c r="TN154" s="15"/>
+      <c r="TO154" s="15"/>
+      <c r="TP154" s="15"/>
+      <c r="TQ154" s="15"/>
+      <c r="TR154" s="15"/>
+      <c r="TS154" s="15"/>
+      <c r="TT154" s="15"/>
+      <c r="TU154" s="15"/>
+      <c r="TV154" s="15"/>
+      <c r="TW154" s="15"/>
+      <c r="TX154" s="15"/>
+      <c r="TY154" s="15"/>
+      <c r="TZ154" s="15"/>
+      <c r="UA154" s="15"/>
+      <c r="UB154" s="15"/>
+      <c r="UC154" s="15"/>
+      <c r="UD154" s="15"/>
+      <c r="UE154" s="15"/>
+      <c r="UF154" s="15"/>
+      <c r="UG154" s="15"/>
+      <c r="UH154" s="15"/>
+      <c r="UI154" s="15"/>
+      <c r="UJ154" s="15"/>
+      <c r="UK154" s="15"/>
+      <c r="UL154" s="15"/>
+      <c r="UM154" s="15"/>
+      <c r="UN154" s="15"/>
+      <c r="UO154" s="15"/>
+      <c r="UP154" s="15"/>
+      <c r="UQ154" s="15"/>
+      <c r="UR154" s="15"/>
+      <c r="US154" s="15"/>
+      <c r="UT154" s="15"/>
+      <c r="UU154" s="15"/>
+      <c r="UV154" s="15"/>
+      <c r="UW154" s="15"/>
+      <c r="UX154" s="15"/>
+      <c r="UY154" s="15"/>
+      <c r="UZ154" s="15"/>
+      <c r="VA154" s="15"/>
+      <c r="VB154" s="15"/>
+      <c r="VC154" s="15"/>
+      <c r="VD154" s="15"/>
+      <c r="VE154" s="15"/>
+      <c r="VF154" s="15"/>
+      <c r="VG154" s="15"/>
+      <c r="VH154" s="15"/>
+      <c r="VI154" s="15"/>
+      <c r="VJ154" s="15"/>
+      <c r="VK154" s="15"/>
+      <c r="VL154" s="15"/>
+      <c r="VM154" s="15"/>
+      <c r="VN154" s="15"/>
+      <c r="VO154" s="15"/>
+      <c r="VP154" s="15"/>
+      <c r="VQ154" s="15"/>
+      <c r="VR154" s="15"/>
+      <c r="VS154" s="15"/>
+      <c r="VT154" s="15"/>
+      <c r="VU154" s="15"/>
+      <c r="VV154" s="15"/>
+      <c r="VW154" s="15"/>
+      <c r="VX154" s="15"/>
+      <c r="VY154" s="15"/>
+      <c r="VZ154" s="15"/>
+      <c r="WA154" s="15"/>
+      <c r="WB154" s="15"/>
+      <c r="WC154" s="15"/>
+      <c r="WD154" s="15"/>
+      <c r="WE154" s="15"/>
+      <c r="WF154" s="15"/>
+      <c r="WG154" s="15"/>
+      <c r="WH154" s="15"/>
+      <c r="WI154" s="15"/>
+      <c r="WJ154" s="15"/>
+      <c r="WK154" s="15"/>
+      <c r="WL154" s="15"/>
+      <c r="WM154" s="15"/>
+      <c r="WN154" s="15"/>
+      <c r="WO154" s="15"/>
+      <c r="WP154" s="15"/>
+      <c r="WQ154" s="15"/>
+      <c r="WR154" s="15"/>
+      <c r="WS154" s="15"/>
+      <c r="WT154" s="15"/>
+      <c r="WU154" s="15"/>
+      <c r="WV154" s="15"/>
+      <c r="WW154" s="15"/>
+      <c r="WX154" s="15"/>
+      <c r="WY154" s="15"/>
+      <c r="WZ154" s="15"/>
+      <c r="XA154" s="15"/>
+      <c r="XB154" s="15"/>
+      <c r="XC154" s="15"/>
+      <c r="XD154" s="15"/>
+      <c r="XE154" s="15"/>
+      <c r="XF154" s="15"/>
+      <c r="XG154" s="15"/>
+      <c r="XH154" s="15"/>
+      <c r="XI154" s="15"/>
+      <c r="XJ154" s="15"/>
+      <c r="XK154" s="15"/>
+      <c r="XL154" s="15"/>
+      <c r="XM154" s="15"/>
+      <c r="XN154" s="15"/>
+      <c r="XO154" s="15"/>
+      <c r="XP154" s="15"/>
+      <c r="XQ154" s="15"/>
+      <c r="XR154" s="15"/>
+      <c r="XS154" s="15"/>
+      <c r="XT154" s="15"/>
+      <c r="XU154" s="15"/>
+      <c r="XV154" s="15"/>
+      <c r="XW154" s="15"/>
+      <c r="XX154" s="15"/>
+      <c r="XY154" s="15"/>
+      <c r="XZ154" s="15"/>
+      <c r="YA154" s="15"/>
+      <c r="YB154" s="15"/>
+      <c r="YC154" s="15"/>
+      <c r="YD154" s="15"/>
+      <c r="YE154" s="15"/>
+      <c r="YF154" s="15"/>
+      <c r="YG154" s="15"/>
+      <c r="YH154" s="15"/>
+      <c r="YI154" s="15"/>
+      <c r="YJ154" s="15"/>
+      <c r="YK154" s="15"/>
+      <c r="YL154" s="15"/>
+      <c r="YM154" s="15"/>
+      <c r="YN154" s="15"/>
+      <c r="YO154" s="15"/>
+      <c r="YP154" s="15"/>
+      <c r="YQ154" s="15"/>
+      <c r="YR154" s="15"/>
+      <c r="YS154" s="15"/>
+      <c r="YT154" s="15"/>
+      <c r="YU154" s="15"/>
+      <c r="YV154" s="15"/>
+      <c r="YW154" s="15"/>
+      <c r="YX154" s="15"/>
+      <c r="YY154" s="15"/>
+      <c r="YZ154" s="15"/>
+      <c r="ZA154" s="15"/>
+      <c r="ZB154" s="15"/>
+      <c r="ZC154" s="15"/>
+      <c r="ZD154" s="15"/>
+      <c r="ZE154" s="15"/>
+      <c r="ZF154" s="15"/>
+      <c r="ZG154" s="15"/>
+      <c r="ZH154" s="15"/>
+      <c r="ZI154" s="15"/>
+      <c r="ZJ154" s="15"/>
+      <c r="ZK154" s="15"/>
+      <c r="ZL154" s="15"/>
+      <c r="ZM154" s="15"/>
+      <c r="ZN154" s="15"/>
+      <c r="ZO154" s="15"/>
+      <c r="ZP154" s="15"/>
+      <c r="ZQ154" s="15"/>
+      <c r="ZR154" s="15"/>
+      <c r="ZS154" s="15"/>
+      <c r="ZT154" s="15"/>
+      <c r="ZU154" s="15"/>
+      <c r="ZV154" s="15"/>
+      <c r="ZW154" s="15"/>
+      <c r="ZX154" s="15"/>
+      <c r="ZY154" s="15"/>
+      <c r="ZZ154" s="15"/>
+      <c r="AAA154" s="15"/>
+      <c r="AAB154" s="15"/>
+      <c r="AAC154" s="15"/>
+      <c r="AAD154" s="15"/>
+      <c r="AAE154" s="15"/>
+      <c r="AAF154" s="15"/>
+      <c r="AAG154" s="15"/>
+      <c r="AAH154" s="15"/>
+      <c r="AAI154" s="15"/>
+      <c r="AAJ154" s="15"/>
+      <c r="AAK154" s="15"/>
+      <c r="AAL154" s="15"/>
+      <c r="AAM154" s="15"/>
+      <c r="AAN154" s="15"/>
+      <c r="AAO154" s="15"/>
+      <c r="AAP154" s="15"/>
+      <c r="AAQ154" s="15"/>
+      <c r="AAR154" s="15"/>
+      <c r="AAS154" s="15"/>
+      <c r="AAT154" s="15"/>
+      <c r="AAU154" s="15"/>
+      <c r="AAV154" s="15"/>
+      <c r="AAW154" s="15"/>
+      <c r="AAX154" s="15"/>
+      <c r="AAY154" s="15"/>
+      <c r="AAZ154" s="15"/>
+      <c r="ABA154" s="15"/>
+      <c r="ABB154" s="15"/>
+      <c r="ABC154" s="15"/>
+      <c r="ABD154" s="15"/>
+      <c r="ABE154" s="15"/>
+      <c r="ABF154" s="15"/>
+      <c r="ABG154" s="15"/>
+      <c r="ABH154" s="15"/>
+      <c r="ABI154" s="15"/>
+      <c r="ABJ154" s="15"/>
+      <c r="ABK154" s="15"/>
+      <c r="ABL154" s="15"/>
+      <c r="ABM154" s="15"/>
+      <c r="ABN154" s="15"/>
+      <c r="ABO154" s="15"/>
+      <c r="ABP154" s="15"/>
+      <c r="ABQ154" s="15"/>
+      <c r="ABR154" s="15"/>
+      <c r="ABS154" s="15"/>
+      <c r="ABT154" s="15"/>
+      <c r="ABU154" s="15"/>
+      <c r="ABV154" s="15"/>
+      <c r="ABW154" s="15"/>
+      <c r="ABX154" s="15"/>
+      <c r="ABY154" s="15"/>
+      <c r="ABZ154" s="15"/>
+      <c r="ACA154" s="15"/>
+      <c r="ACB154" s="15"/>
+      <c r="ACC154" s="15"/>
+      <c r="ACD154" s="15"/>
+      <c r="ACE154" s="15"/>
+      <c r="ACF154" s="15"/>
+      <c r="ACG154" s="15"/>
+      <c r="ACH154" s="15"/>
+      <c r="ACI154" s="15"/>
+      <c r="ACJ154" s="15"/>
+      <c r="ACK154" s="15"/>
+      <c r="ACL154" s="15"/>
+      <c r="ACM154" s="15"/>
+      <c r="ACN154" s="15"/>
+      <c r="ACO154" s="15"/>
+      <c r="ACP154" s="15"/>
+      <c r="ACQ154" s="15"/>
+      <c r="ACR154" s="15"/>
+      <c r="ACS154" s="15"/>
+      <c r="ACT154" s="15"/>
+      <c r="ACU154" s="15"/>
+      <c r="ACV154" s="15"/>
+      <c r="ACW154" s="15"/>
+      <c r="ACX154" s="15"/>
+      <c r="ACY154" s="15"/>
+      <c r="ACZ154" s="15"/>
+      <c r="ADA154" s="15"/>
+      <c r="ADB154" s="15"/>
+      <c r="ADC154" s="15"/>
+      <c r="ADD154" s="15"/>
+      <c r="ADE154" s="15"/>
+      <c r="ADF154" s="15"/>
+      <c r="ADG154" s="15"/>
+      <c r="ADH154" s="15"/>
+      <c r="ADI154" s="15"/>
+      <c r="ADJ154" s="15"/>
+      <c r="ADK154" s="15"/>
+      <c r="ADL154" s="15"/>
+      <c r="ADM154" s="15"/>
+      <c r="ADN154" s="15"/>
+      <c r="ADO154" s="15"/>
+      <c r="ADP154" s="15"/>
+      <c r="ADQ154" s="15"/>
+      <c r="ADR154" s="15"/>
+      <c r="ADS154" s="15"/>
+      <c r="ADT154" s="15"/>
+      <c r="ADU154" s="15"/>
+      <c r="ADV154" s="15"/>
+      <c r="ADW154" s="15"/>
+      <c r="ADX154" s="15"/>
+      <c r="ADY154" s="15"/>
+      <c r="ADZ154" s="15"/>
+      <c r="AEA154" s="15"/>
+      <c r="AEB154" s="15"/>
+      <c r="AEC154" s="15"/>
+      <c r="AED154" s="15"/>
+      <c r="AEE154" s="15"/>
+      <c r="AEF154" s="15"/>
+      <c r="AEG154" s="15"/>
+      <c r="AEH154" s="15"/>
+      <c r="AEI154" s="15"/>
+      <c r="AEJ154" s="15"/>
+      <c r="AEK154" s="15"/>
+      <c r="AEL154" s="15"/>
+      <c r="AEM154" s="15"/>
+      <c r="AEN154" s="15"/>
+      <c r="AEO154" s="15"/>
+      <c r="AEP154" s="15"/>
+      <c r="AEQ154" s="15"/>
+      <c r="AER154" s="15"/>
+      <c r="AES154" s="15"/>
+      <c r="AET154" s="15"/>
+      <c r="AEU154" s="15"/>
+      <c r="AEV154" s="15"/>
+      <c r="AEW154" s="15"/>
+      <c r="AEX154" s="15"/>
+      <c r="AEY154" s="15"/>
+      <c r="AEZ154" s="15"/>
+      <c r="AFA154" s="15"/>
+      <c r="AFB154" s="15"/>
+      <c r="AFC154" s="15"/>
+      <c r="AFD154" s="15"/>
+      <c r="AFE154" s="15"/>
+      <c r="AFF154" s="15"/>
+      <c r="AFG154" s="15"/>
+      <c r="AFH154" s="15"/>
+      <c r="AFI154" s="15"/>
+      <c r="AFJ154" s="15"/>
+      <c r="AFK154" s="15"/>
+      <c r="AFL154" s="15"/>
+      <c r="AFM154" s="15"/>
+      <c r="AFN154" s="15"/>
+      <c r="AFO154" s="15"/>
+      <c r="AFP154" s="15"/>
+      <c r="AFQ154" s="15"/>
+      <c r="AFR154" s="15"/>
+      <c r="AFS154" s="15"/>
+      <c r="AFT154" s="15"/>
+      <c r="AFU154" s="15"/>
+      <c r="AFV154" s="15"/>
+      <c r="AFW154" s="15"/>
+      <c r="AFX154" s="15"/>
+      <c r="AFY154" s="15"/>
+      <c r="AFZ154" s="15"/>
+      <c r="AGA154" s="15"/>
+      <c r="AGB154" s="15"/>
+      <c r="AGC154" s="15"/>
+      <c r="AGD154" s="15"/>
+      <c r="AGE154" s="15"/>
+      <c r="AGF154" s="15"/>
+      <c r="AGG154" s="15"/>
+      <c r="AGH154" s="15"/>
+      <c r="AGI154" s="15"/>
+      <c r="AGJ154" s="15"/>
+      <c r="AGK154" s="15"/>
+      <c r="AGL154" s="15"/>
+      <c r="AGM154" s="15"/>
+      <c r="AGN154" s="15"/>
+      <c r="AGO154" s="15"/>
+      <c r="AGP154" s="15"/>
+      <c r="AGQ154" s="15"/>
+      <c r="AGR154" s="15"/>
+      <c r="AGS154" s="15"/>
+      <c r="AGT154" s="15"/>
+      <c r="AGU154" s="15"/>
+      <c r="AGV154" s="15"/>
+      <c r="AGW154" s="15"/>
+      <c r="AGX154" s="15"/>
+      <c r="AGY154" s="15"/>
+      <c r="AGZ154" s="15"/>
+      <c r="AHA154" s="15"/>
+      <c r="AHB154" s="15"/>
+      <c r="AHC154" s="15"/>
+      <c r="AHD154" s="15"/>
+      <c r="AHE154" s="15"/>
+      <c r="AHF154" s="15"/>
+      <c r="AHG154" s="15"/>
+      <c r="AHH154" s="15"/>
+      <c r="AHI154" s="15"/>
+      <c r="AHJ154" s="15"/>
+      <c r="AHK154" s="15"/>
+      <c r="AHL154" s="15"/>
+      <c r="AHM154" s="15"/>
+      <c r="AHN154" s="15"/>
+      <c r="AHO154" s="15"/>
+      <c r="AHP154" s="15"/>
+      <c r="AHQ154" s="15"/>
+      <c r="AHR154" s="15"/>
+      <c r="AHS154" s="15"/>
+      <c r="AHT154" s="15"/>
+      <c r="AHU154" s="15"/>
+      <c r="AHV154" s="15"/>
+      <c r="AHW154" s="15"/>
+      <c r="AHX154" s="15"/>
+      <c r="AHY154" s="15"/>
+      <c r="AHZ154" s="15"/>
+      <c r="AIA154" s="15"/>
+      <c r="AIB154" s="15"/>
+      <c r="AIC154" s="15"/>
+      <c r="AID154" s="15"/>
+      <c r="AIE154" s="15"/>
+      <c r="AIF154" s="15"/>
+      <c r="AIG154" s="15"/>
+      <c r="AIH154" s="15"/>
+      <c r="AII154" s="15"/>
+      <c r="AIJ154" s="15"/>
+      <c r="AIK154" s="15"/>
+      <c r="AIL154" s="15"/>
+      <c r="AIM154" s="15"/>
+      <c r="AIN154" s="15"/>
+      <c r="AIO154" s="15"/>
+      <c r="AIP154" s="15"/>
+      <c r="AIQ154" s="15"/>
+      <c r="AIR154" s="15"/>
+      <c r="AIS154" s="15"/>
+      <c r="AIT154" s="15"/>
+      <c r="AIU154" s="15"/>
+      <c r="AIV154" s="15"/>
+      <c r="AIW154" s="15"/>
+      <c r="AIX154" s="15"/>
+      <c r="AIY154" s="15"/>
+      <c r="AIZ154" s="15"/>
+      <c r="AJA154" s="15"/>
+      <c r="AJB154" s="15"/>
+      <c r="AJC154" s="15"/>
+      <c r="AJD154" s="15"/>
+      <c r="AJE154" s="15"/>
+      <c r="AJF154" s="15"/>
+      <c r="AJG154" s="15"/>
+      <c r="AJH154" s="15"/>
+      <c r="AJI154" s="15"/>
+      <c r="AJJ154" s="15"/>
+      <c r="AJK154" s="15"/>
+      <c r="AJL154" s="15"/>
+      <c r="AJM154" s="15"/>
+      <c r="AJN154" s="15"/>
+      <c r="AJO154" s="15"/>
+      <c r="AJP154" s="15"/>
+      <c r="AJQ154" s="15"/>
+      <c r="AJR154" s="15"/>
+      <c r="AJS154" s="15"/>
+      <c r="AJT154" s="15"/>
+      <c r="AJU154" s="15"/>
+      <c r="AJV154" s="15"/>
+      <c r="AJW154" s="15"/>
+      <c r="AJX154" s="15"/>
+      <c r="AJY154" s="15"/>
+      <c r="AJZ154" s="15"/>
+      <c r="AKA154" s="15"/>
+      <c r="AKB154" s="15"/>
+      <c r="AKC154" s="15"/>
+      <c r="AKD154" s="15"/>
+      <c r="AKE154" s="15"/>
+      <c r="AKF154" s="15"/>
+      <c r="AKG154" s="15"/>
+      <c r="AKH154" s="15"/>
+      <c r="AKI154" s="15"/>
+      <c r="AKJ154" s="15"/>
+      <c r="AKK154" s="15"/>
+      <c r="AKL154" s="15"/>
+      <c r="AKM154" s="15"/>
+      <c r="AKN154" s="15"/>
+      <c r="AKO154" s="15"/>
+      <c r="AKP154" s="15"/>
+      <c r="AKQ154" s="15"/>
+      <c r="AKR154" s="15"/>
+      <c r="AKS154" s="15"/>
+      <c r="AKT154" s="15"/>
+      <c r="AKU154" s="15"/>
+      <c r="AKV154" s="15"/>
+      <c r="AKW154" s="15"/>
+      <c r="AKX154" s="15"/>
+      <c r="AKY154" s="15"/>
+      <c r="AKZ154" s="15"/>
+      <c r="ALA154" s="15"/>
+      <c r="ALB154" s="15"/>
+      <c r="ALC154" s="15"/>
+      <c r="ALD154" s="15"/>
+      <c r="ALE154" s="15"/>
+      <c r="ALF154" s="15"/>
+      <c r="ALG154" s="15"/>
+      <c r="ALH154" s="15"/>
+      <c r="ALI154" s="15"/>
+      <c r="ALJ154" s="15"/>
+      <c r="ALK154" s="15"/>
+      <c r="ALL154" s="15"/>
+      <c r="ALM154" s="15"/>
+      <c r="ALN154" s="15"/>
+      <c r="ALO154" s="15"/>
+      <c r="ALP154" s="15"/>
+      <c r="ALQ154" s="15"/>
+      <c r="ALR154" s="15"/>
+      <c r="ALS154" s="15"/>
+      <c r="ALT154" s="15"/>
+      <c r="ALU154" s="15"/>
+      <c r="ALV154" s="15"/>
+      <c r="ALW154" s="15"/>
+      <c r="ALX154" s="15"/>
+      <c r="ALY154" s="15"/>
+      <c r="ALZ154" s="15"/>
+      <c r="AMA154" s="15"/>
+      <c r="AMB154" s="15"/>
+      <c r="AMC154" s="15"/>
+      <c r="AMD154" s="15"/>
+      <c r="AME154" s="15"/>
+      <c r="AMF154" s="15"/>
+      <c r="AMG154" s="15"/>
+      <c r="AMH154" s="15"/>
+      <c r="AMI154" s="15"/>
+      <c r="AMJ154" s="15"/>
     </row>
     <row r="155" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="15"/>
@@ -2675,53 +3694,88 @@
       <c r="P157" s="36"/>
     </row>
     <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B158" s="35"/>
-      <c r="C158" s="35"/>
-      <c r="D158" s="38"/>
-      <c r="E158" s="36"/>
-      <c r="G158" s="36"/>
-      <c r="L158" s="35"/>
-      <c r="M158" s="35"/>
-      <c r="N158" s="35"/>
-      <c r="O158" s="38"/>
-      <c r="P158" s="36"/>
+      <c r="B158" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C158" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D158" s="21"/>
+      <c r="E158" s="24"/>
+      <c r="F158" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="G158" s="39"/>
+      <c r="H158" s="39"/>
+      <c r="I158" s="39"/>
+      <c r="L158" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="M158" s="29"/>
+      <c r="N158" s="21"/>
+      <c r="O158" s="29"/>
+      <c r="P158" s="21"/>
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B159" s="35"/>
-      <c r="C159" s="35"/>
-      <c r="D159" s="38"/>
-      <c r="E159" s="36"/>
-      <c r="G159" s="36"/>
-      <c r="L159" s="35"/>
-      <c r="M159" s="35"/>
-      <c r="N159" s="35"/>
-      <c r="O159" s="38"/>
-      <c r="P159" s="36"/>
+      <c r="B159" s="21"/>
+      <c r="C159" s="29"/>
+      <c r="D159" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E159" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F159" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="G159" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="H159" s="39"/>
+      <c r="I159" s="39"/>
+      <c r="L159" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="M159" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="N159" s="21"/>
+      <c r="O159" s="29"/>
+      <c r="P159" s="21"/>
     </row>
     <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B160" s="35"/>
-      <c r="C160" s="35"/>
-      <c r="D160" s="38"/>
-      <c r="E160" s="36"/>
-      <c r="G160" s="36"/>
-      <c r="L160" s="35"/>
-      <c r="M160" s="35"/>
-      <c r="N160" s="35"/>
-      <c r="O160" s="38"/>
-      <c r="P160" s="36"/>
+      <c r="B160" s="0"/>
+      <c r="C160" s="0"/>
+      <c r="D160" s="0"/>
+      <c r="E160" s="0"/>
+      <c r="F160" s="0"/>
+      <c r="G160" s="0"/>
+      <c r="H160" s="0"/>
+      <c r="I160" s="0"/>
+      <c r="J160" s="0"/>
+      <c r="K160" s="0"/>
+      <c r="L160" s="0"/>
+      <c r="M160" s="0"/>
+      <c r="N160" s="0"/>
+      <c r="O160" s="0"/>
+      <c r="P160" s="0"/>
     </row>
     <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B161" s="35"/>
-      <c r="C161" s="35"/>
-      <c r="D161" s="38"/>
-      <c r="E161" s="36"/>
-      <c r="F161" s="36"/>
-      <c r="G161" s="36"/>
-      <c r="L161" s="35"/>
-      <c r="M161" s="35"/>
-      <c r="N161" s="35"/>
-      <c r="O161" s="38"/>
-      <c r="P161" s="36"/>
+      <c r="B161" s="0"/>
+      <c r="C161" s="0"/>
+      <c r="D161" s="0"/>
+      <c r="E161" s="0"/>
+      <c r="F161" s="0"/>
+      <c r="G161" s="0"/>
+      <c r="H161" s="0"/>
+      <c r="I161" s="0"/>
+      <c r="J161" s="0"/>
+      <c r="K161" s="0"/>
+      <c r="L161" s="0"/>
+      <c r="M161" s="0"/>
+      <c r="N161" s="0"/>
+      <c r="O161" s="0"/>
+      <c r="P161" s="0"/>
     </row>
     <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="21"/>
@@ -3191,10 +4245,10 @@
     <row r="193" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="15"/>
       <c r="B193" s="16" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C193" s="17" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D193" s="16"/>
       <c r="E193" s="17"/>
@@ -3213,14 +4267,14 @@
     <row r="194" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="23"/>
       <c r="B194" s="35" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C194" s="35" t="s">
         <v>51</v>
       </c>
       <c r="D194" s="38"/>
       <c r="F194" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="M194" s="35"/>
       <c r="N194" s="35"/>
@@ -3237,7 +4291,7 @@
         <v>54</v>
       </c>
       <c r="F195" s="36" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G195" s="36" t="s">
         <v>4</v>
@@ -3247,7 +4301,7 @@
       <c r="J195" s="37"/>
       <c r="K195" s="37"/>
       <c r="L195" s="35" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M195" s="35"/>
       <c r="N195" s="35"/>
@@ -3259,17 +4313,9 @@
       <c r="B196" s="35"/>
       <c r="C196" s="35"/>
       <c r="D196" s="38"/>
-      <c r="E196" s="36"/>
-      <c r="G196" s="36"/>
-      <c r="H196" s="36"/>
-      <c r="I196" s="36"/>
-      <c r="J196" s="37"/>
-      <c r="K196" s="37"/>
-      <c r="L196" s="35"/>
       <c r="M196" s="35"/>
       <c r="N196" s="35"/>
       <c r="O196" s="38"/>
-      <c r="P196" s="36"/>
     </row>
     <row r="197" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="23"/>
@@ -3277,6 +4323,7 @@
       <c r="C197" s="35"/>
       <c r="D197" s="38"/>
       <c r="E197" s="36"/>
+      <c r="F197" s="36"/>
       <c r="G197" s="36"/>
       <c r="H197" s="36"/>
       <c r="I197" s="36"/>
@@ -3288,1031 +4335,14 @@
       <c r="O197" s="38"/>
       <c r="P197" s="36"/>
     </row>
-    <row r="198" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="23"/>
       <c r="B198" s="35"/>
       <c r="C198" s="35"/>
       <c r="D198" s="38"/>
-      <c r="E198" s="36"/>
-      <c r="F198" s="1"/>
-      <c r="G198" s="36"/>
-      <c r="H198" s="36"/>
-      <c r="I198" s="36"/>
-      <c r="J198" s="37"/>
-      <c r="K198" s="37"/>
-      <c r="L198" s="35"/>
       <c r="M198" s="35"/>
       <c r="N198" s="35"/>
       <c r="O198" s="38"/>
-      <c r="P198" s="36"/>
-      <c r="Q198" s="1"/>
-      <c r="R198" s="1"/>
-      <c r="S198" s="1"/>
-      <c r="T198" s="1"/>
-      <c r="U198" s="1"/>
-      <c r="V198" s="1"/>
-      <c r="W198" s="1"/>
-      <c r="X198" s="1"/>
-      <c r="Y198" s="1"/>
-      <c r="Z198" s="1"/>
-      <c r="AA198" s="1"/>
-      <c r="AB198" s="1"/>
-      <c r="AC198" s="1"/>
-      <c r="AD198" s="1"/>
-      <c r="AE198" s="1"/>
-      <c r="AF198" s="1"/>
-      <c r="AG198" s="1"/>
-      <c r="AH198" s="1"/>
-      <c r="AI198" s="1"/>
-      <c r="AJ198" s="1"/>
-      <c r="AK198" s="1"/>
-      <c r="AL198" s="1"/>
-      <c r="AM198" s="1"/>
-      <c r="AN198" s="1"/>
-      <c r="AO198" s="1"/>
-      <c r="AP198" s="1"/>
-      <c r="AQ198" s="1"/>
-      <c r="AR198" s="1"/>
-      <c r="AS198" s="1"/>
-      <c r="AT198" s="1"/>
-      <c r="AU198" s="1"/>
-      <c r="AV198" s="1"/>
-      <c r="AW198" s="1"/>
-      <c r="AX198" s="1"/>
-      <c r="AY198" s="1"/>
-      <c r="AZ198" s="1"/>
-      <c r="BA198" s="1"/>
-      <c r="BB198" s="1"/>
-      <c r="BC198" s="1"/>
-      <c r="BD198" s="1"/>
-      <c r="BE198" s="1"/>
-      <c r="BF198" s="1"/>
-      <c r="BG198" s="1"/>
-      <c r="BH198" s="1"/>
-      <c r="BI198" s="1"/>
-      <c r="BJ198" s="1"/>
-      <c r="BK198" s="1"/>
-      <c r="BL198" s="1"/>
-      <c r="BM198" s="1"/>
-      <c r="BN198" s="1"/>
-      <c r="BO198" s="1"/>
-      <c r="BP198" s="1"/>
-      <c r="BQ198" s="1"/>
-      <c r="BR198" s="1"/>
-      <c r="BS198" s="1"/>
-      <c r="BT198" s="1"/>
-      <c r="BU198" s="1"/>
-      <c r="BV198" s="1"/>
-      <c r="BW198" s="1"/>
-      <c r="BX198" s="1"/>
-      <c r="BY198" s="1"/>
-      <c r="BZ198" s="1"/>
-      <c r="CA198" s="1"/>
-      <c r="CB198" s="1"/>
-      <c r="CC198" s="1"/>
-      <c r="CD198" s="1"/>
-      <c r="CE198" s="1"/>
-      <c r="CF198" s="1"/>
-      <c r="CG198" s="1"/>
-      <c r="CH198" s="1"/>
-      <c r="CI198" s="1"/>
-      <c r="CJ198" s="1"/>
-      <c r="CK198" s="1"/>
-      <c r="CL198" s="1"/>
-      <c r="CM198" s="1"/>
-      <c r="CN198" s="1"/>
-      <c r="CO198" s="1"/>
-      <c r="CP198" s="1"/>
-      <c r="CQ198" s="1"/>
-      <c r="CR198" s="1"/>
-      <c r="CS198" s="1"/>
-      <c r="CT198" s="1"/>
-      <c r="CU198" s="1"/>
-      <c r="CV198" s="1"/>
-      <c r="CW198" s="1"/>
-      <c r="CX198" s="1"/>
-      <c r="CY198" s="1"/>
-      <c r="CZ198" s="1"/>
-      <c r="DA198" s="1"/>
-      <c r="DB198" s="1"/>
-      <c r="DC198" s="1"/>
-      <c r="DD198" s="1"/>
-      <c r="DE198" s="1"/>
-      <c r="DF198" s="1"/>
-      <c r="DG198" s="1"/>
-      <c r="DH198" s="1"/>
-      <c r="DI198" s="1"/>
-      <c r="DJ198" s="1"/>
-      <c r="DK198" s="1"/>
-      <c r="DL198" s="1"/>
-      <c r="DM198" s="1"/>
-      <c r="DN198" s="1"/>
-      <c r="DO198" s="1"/>
-      <c r="DP198" s="1"/>
-      <c r="DQ198" s="1"/>
-      <c r="DR198" s="1"/>
-      <c r="DS198" s="1"/>
-      <c r="DT198" s="1"/>
-      <c r="DU198" s="1"/>
-      <c r="DV198" s="1"/>
-      <c r="DW198" s="1"/>
-      <c r="DX198" s="1"/>
-      <c r="DY198" s="1"/>
-      <c r="DZ198" s="1"/>
-      <c r="EA198" s="1"/>
-      <c r="EB198" s="1"/>
-      <c r="EC198" s="1"/>
-      <c r="ED198" s="1"/>
-      <c r="EE198" s="1"/>
-      <c r="EF198" s="1"/>
-      <c r="EG198" s="1"/>
-      <c r="EH198" s="1"/>
-      <c r="EI198" s="1"/>
-      <c r="EJ198" s="1"/>
-      <c r="EK198" s="1"/>
-      <c r="EL198" s="1"/>
-      <c r="EM198" s="1"/>
-      <c r="EN198" s="1"/>
-      <c r="EO198" s="1"/>
-      <c r="EP198" s="1"/>
-      <c r="EQ198" s="1"/>
-      <c r="ER198" s="1"/>
-      <c r="ES198" s="1"/>
-      <c r="ET198" s="1"/>
-      <c r="EU198" s="1"/>
-      <c r="EV198" s="1"/>
-      <c r="EW198" s="1"/>
-      <c r="EX198" s="1"/>
-      <c r="EY198" s="1"/>
-      <c r="EZ198" s="1"/>
-      <c r="FA198" s="1"/>
-      <c r="FB198" s="1"/>
-      <c r="FC198" s="1"/>
-      <c r="FD198" s="1"/>
-      <c r="FE198" s="1"/>
-      <c r="FF198" s="1"/>
-      <c r="FG198" s="1"/>
-      <c r="FH198" s="1"/>
-      <c r="FI198" s="1"/>
-      <c r="FJ198" s="1"/>
-      <c r="FK198" s="1"/>
-      <c r="FL198" s="1"/>
-      <c r="FM198" s="1"/>
-      <c r="FN198" s="1"/>
-      <c r="FO198" s="1"/>
-      <c r="FP198" s="1"/>
-      <c r="FQ198" s="1"/>
-      <c r="FR198" s="1"/>
-      <c r="FS198" s="1"/>
-      <c r="FT198" s="1"/>
-      <c r="FU198" s="1"/>
-      <c r="FV198" s="1"/>
-      <c r="FW198" s="1"/>
-      <c r="FX198" s="1"/>
-      <c r="FY198" s="1"/>
-      <c r="FZ198" s="1"/>
-      <c r="GA198" s="1"/>
-      <c r="GB198" s="1"/>
-      <c r="GC198" s="1"/>
-      <c r="GD198" s="1"/>
-      <c r="GE198" s="1"/>
-      <c r="GF198" s="1"/>
-      <c r="GG198" s="1"/>
-      <c r="GH198" s="1"/>
-      <c r="GI198" s="1"/>
-      <c r="GJ198" s="1"/>
-      <c r="GK198" s="1"/>
-      <c r="GL198" s="1"/>
-      <c r="GM198" s="1"/>
-      <c r="GN198" s="1"/>
-      <c r="GO198" s="1"/>
-      <c r="GP198" s="1"/>
-      <c r="GQ198" s="1"/>
-      <c r="GR198" s="1"/>
-      <c r="GS198" s="1"/>
-      <c r="GT198" s="1"/>
-      <c r="GU198" s="1"/>
-      <c r="GV198" s="1"/>
-      <c r="GW198" s="1"/>
-      <c r="GX198" s="1"/>
-      <c r="GY198" s="1"/>
-      <c r="GZ198" s="1"/>
-      <c r="HA198" s="1"/>
-      <c r="HB198" s="1"/>
-      <c r="HC198" s="1"/>
-      <c r="HD198" s="1"/>
-      <c r="HE198" s="1"/>
-      <c r="HF198" s="1"/>
-      <c r="HG198" s="1"/>
-      <c r="HH198" s="1"/>
-      <c r="HI198" s="1"/>
-      <c r="HJ198" s="1"/>
-      <c r="HK198" s="1"/>
-      <c r="HL198" s="1"/>
-      <c r="HM198" s="1"/>
-      <c r="HN198" s="1"/>
-      <c r="HO198" s="1"/>
-      <c r="HP198" s="1"/>
-      <c r="HQ198" s="1"/>
-      <c r="HR198" s="1"/>
-      <c r="HS198" s="1"/>
-      <c r="HT198" s="1"/>
-      <c r="HU198" s="1"/>
-      <c r="HV198" s="1"/>
-      <c r="HW198" s="1"/>
-      <c r="HX198" s="1"/>
-      <c r="HY198" s="1"/>
-      <c r="HZ198" s="1"/>
-      <c r="IA198" s="1"/>
-      <c r="IB198" s="1"/>
-      <c r="IC198" s="1"/>
-      <c r="ID198" s="1"/>
-      <c r="IE198" s="1"/>
-      <c r="IF198" s="1"/>
-      <c r="IG198" s="1"/>
-      <c r="IH198" s="1"/>
-      <c r="II198" s="1"/>
-      <c r="IJ198" s="1"/>
-      <c r="IK198" s="1"/>
-      <c r="IL198" s="1"/>
-      <c r="IM198" s="1"/>
-      <c r="IN198" s="1"/>
-      <c r="IO198" s="1"/>
-      <c r="IP198" s="1"/>
-      <c r="IQ198" s="1"/>
-      <c r="IR198" s="1"/>
-      <c r="IS198" s="1"/>
-      <c r="IT198" s="1"/>
-      <c r="IU198" s="1"/>
-      <c r="IV198" s="1"/>
-      <c r="IW198" s="1"/>
-      <c r="IX198" s="1"/>
-      <c r="IY198" s="1"/>
-      <c r="IZ198" s="1"/>
-      <c r="JA198" s="1"/>
-      <c r="JB198" s="1"/>
-      <c r="JC198" s="1"/>
-      <c r="JD198" s="1"/>
-      <c r="JE198" s="1"/>
-      <c r="JF198" s="1"/>
-      <c r="JG198" s="1"/>
-      <c r="JH198" s="1"/>
-      <c r="JI198" s="1"/>
-      <c r="JJ198" s="1"/>
-      <c r="JK198" s="1"/>
-      <c r="JL198" s="1"/>
-      <c r="JM198" s="1"/>
-      <c r="JN198" s="1"/>
-      <c r="JO198" s="1"/>
-      <c r="JP198" s="1"/>
-      <c r="JQ198" s="1"/>
-      <c r="JR198" s="1"/>
-      <c r="JS198" s="1"/>
-      <c r="JT198" s="1"/>
-      <c r="JU198" s="1"/>
-      <c r="JV198" s="1"/>
-      <c r="JW198" s="1"/>
-      <c r="JX198" s="1"/>
-      <c r="JY198" s="1"/>
-      <c r="JZ198" s="1"/>
-      <c r="KA198" s="1"/>
-      <c r="KB198" s="1"/>
-      <c r="KC198" s="1"/>
-      <c r="KD198" s="1"/>
-      <c r="KE198" s="1"/>
-      <c r="KF198" s="1"/>
-      <c r="KG198" s="1"/>
-      <c r="KH198" s="1"/>
-      <c r="KI198" s="1"/>
-      <c r="KJ198" s="1"/>
-      <c r="KK198" s="1"/>
-      <c r="KL198" s="1"/>
-      <c r="KM198" s="1"/>
-      <c r="KN198" s="1"/>
-      <c r="KO198" s="1"/>
-      <c r="KP198" s="1"/>
-      <c r="KQ198" s="1"/>
-      <c r="KR198" s="1"/>
-      <c r="KS198" s="1"/>
-      <c r="KT198" s="1"/>
-      <c r="KU198" s="1"/>
-      <c r="KV198" s="1"/>
-      <c r="KW198" s="1"/>
-      <c r="KX198" s="1"/>
-      <c r="KY198" s="1"/>
-      <c r="KZ198" s="1"/>
-      <c r="LA198" s="1"/>
-      <c r="LB198" s="1"/>
-      <c r="LC198" s="1"/>
-      <c r="LD198" s="1"/>
-      <c r="LE198" s="1"/>
-      <c r="LF198" s="1"/>
-      <c r="LG198" s="1"/>
-      <c r="LH198" s="1"/>
-      <c r="LI198" s="1"/>
-      <c r="LJ198" s="1"/>
-      <c r="LK198" s="1"/>
-      <c r="LL198" s="1"/>
-      <c r="LM198" s="1"/>
-      <c r="LN198" s="1"/>
-      <c r="LO198" s="1"/>
-      <c r="LP198" s="1"/>
-      <c r="LQ198" s="1"/>
-      <c r="LR198" s="1"/>
-      <c r="LS198" s="1"/>
-      <c r="LT198" s="1"/>
-      <c r="LU198" s="1"/>
-      <c r="LV198" s="1"/>
-      <c r="LW198" s="1"/>
-      <c r="LX198" s="1"/>
-      <c r="LY198" s="1"/>
-      <c r="LZ198" s="1"/>
-      <c r="MA198" s="1"/>
-      <c r="MB198" s="1"/>
-      <c r="MC198" s="1"/>
-      <c r="MD198" s="1"/>
-      <c r="ME198" s="1"/>
-      <c r="MF198" s="1"/>
-      <c r="MG198" s="1"/>
-      <c r="MH198" s="1"/>
-      <c r="MI198" s="1"/>
-      <c r="MJ198" s="1"/>
-      <c r="MK198" s="1"/>
-      <c r="ML198" s="1"/>
-      <c r="MM198" s="1"/>
-      <c r="MN198" s="1"/>
-      <c r="MO198" s="1"/>
-      <c r="MP198" s="1"/>
-      <c r="MQ198" s="1"/>
-      <c r="MR198" s="1"/>
-      <c r="MS198" s="1"/>
-      <c r="MT198" s="1"/>
-      <c r="MU198" s="1"/>
-      <c r="MV198" s="1"/>
-      <c r="MW198" s="1"/>
-      <c r="MX198" s="1"/>
-      <c r="MY198" s="1"/>
-      <c r="MZ198" s="1"/>
-      <c r="NA198" s="1"/>
-      <c r="NB198" s="1"/>
-      <c r="NC198" s="1"/>
-      <c r="ND198" s="1"/>
-      <c r="NE198" s="1"/>
-      <c r="NF198" s="1"/>
-      <c r="NG198" s="1"/>
-      <c r="NH198" s="1"/>
-      <c r="NI198" s="1"/>
-      <c r="NJ198" s="1"/>
-      <c r="NK198" s="1"/>
-      <c r="NL198" s="1"/>
-      <c r="NM198" s="1"/>
-      <c r="NN198" s="1"/>
-      <c r="NO198" s="1"/>
-      <c r="NP198" s="1"/>
-      <c r="NQ198" s="1"/>
-      <c r="NR198" s="1"/>
-      <c r="NS198" s="1"/>
-      <c r="NT198" s="1"/>
-      <c r="NU198" s="1"/>
-      <c r="NV198" s="1"/>
-      <c r="NW198" s="1"/>
-      <c r="NX198" s="1"/>
-      <c r="NY198" s="1"/>
-      <c r="NZ198" s="1"/>
-      <c r="OA198" s="1"/>
-      <c r="OB198" s="1"/>
-      <c r="OC198" s="1"/>
-      <c r="OD198" s="1"/>
-      <c r="OE198" s="1"/>
-      <c r="OF198" s="1"/>
-      <c r="OG198" s="1"/>
-      <c r="OH198" s="1"/>
-      <c r="OI198" s="1"/>
-      <c r="OJ198" s="1"/>
-      <c r="OK198" s="1"/>
-      <c r="OL198" s="1"/>
-      <c r="OM198" s="1"/>
-      <c r="ON198" s="1"/>
-      <c r="OO198" s="1"/>
-      <c r="OP198" s="1"/>
-      <c r="OQ198" s="1"/>
-      <c r="OR198" s="1"/>
-      <c r="OS198" s="1"/>
-      <c r="OT198" s="1"/>
-      <c r="OU198" s="1"/>
-      <c r="OV198" s="1"/>
-      <c r="OW198" s="1"/>
-      <c r="OX198" s="1"/>
-      <c r="OY198" s="1"/>
-      <c r="OZ198" s="1"/>
-      <c r="PA198" s="1"/>
-      <c r="PB198" s="1"/>
-      <c r="PC198" s="1"/>
-      <c r="PD198" s="1"/>
-      <c r="PE198" s="1"/>
-      <c r="PF198" s="1"/>
-      <c r="PG198" s="1"/>
-      <c r="PH198" s="1"/>
-      <c r="PI198" s="1"/>
-      <c r="PJ198" s="1"/>
-      <c r="PK198" s="1"/>
-      <c r="PL198" s="1"/>
-      <c r="PM198" s="1"/>
-      <c r="PN198" s="1"/>
-      <c r="PO198" s="1"/>
-      <c r="PP198" s="1"/>
-      <c r="PQ198" s="1"/>
-      <c r="PR198" s="1"/>
-      <c r="PS198" s="1"/>
-      <c r="PT198" s="1"/>
-      <c r="PU198" s="1"/>
-      <c r="PV198" s="1"/>
-      <c r="PW198" s="1"/>
-      <c r="PX198" s="1"/>
-      <c r="PY198" s="1"/>
-      <c r="PZ198" s="1"/>
-      <c r="QA198" s="1"/>
-      <c r="QB198" s="1"/>
-      <c r="QC198" s="1"/>
-      <c r="QD198" s="1"/>
-      <c r="QE198" s="1"/>
-      <c r="QF198" s="1"/>
-      <c r="QG198" s="1"/>
-      <c r="QH198" s="1"/>
-      <c r="QI198" s="1"/>
-      <c r="QJ198" s="1"/>
-      <c r="QK198" s="1"/>
-      <c r="QL198" s="1"/>
-      <c r="QM198" s="1"/>
-      <c r="QN198" s="1"/>
-      <c r="QO198" s="1"/>
-      <c r="QP198" s="1"/>
-      <c r="QQ198" s="1"/>
-      <c r="QR198" s="1"/>
-      <c r="QS198" s="1"/>
-      <c r="QT198" s="1"/>
-      <c r="QU198" s="1"/>
-      <c r="QV198" s="1"/>
-      <c r="QW198" s="1"/>
-      <c r="QX198" s="1"/>
-      <c r="QY198" s="1"/>
-      <c r="QZ198" s="1"/>
-      <c r="RA198" s="1"/>
-      <c r="RB198" s="1"/>
-      <c r="RC198" s="1"/>
-      <c r="RD198" s="1"/>
-      <c r="RE198" s="1"/>
-      <c r="RF198" s="1"/>
-      <c r="RG198" s="1"/>
-      <c r="RH198" s="1"/>
-      <c r="RI198" s="1"/>
-      <c r="RJ198" s="1"/>
-      <c r="RK198" s="1"/>
-      <c r="RL198" s="1"/>
-      <c r="RM198" s="1"/>
-      <c r="RN198" s="1"/>
-      <c r="RO198" s="1"/>
-      <c r="RP198" s="1"/>
-      <c r="RQ198" s="1"/>
-      <c r="RR198" s="1"/>
-      <c r="RS198" s="1"/>
-      <c r="RT198" s="1"/>
-      <c r="RU198" s="1"/>
-      <c r="RV198" s="1"/>
-      <c r="RW198" s="1"/>
-      <c r="RX198" s="1"/>
-      <c r="RY198" s="1"/>
-      <c r="RZ198" s="1"/>
-      <c r="SA198" s="1"/>
-      <c r="SB198" s="1"/>
-      <c r="SC198" s="1"/>
-      <c r="SD198" s="1"/>
-      <c r="SE198" s="1"/>
-      <c r="SF198" s="1"/>
-      <c r="SG198" s="1"/>
-      <c r="SH198" s="1"/>
-      <c r="SI198" s="1"/>
-      <c r="SJ198" s="1"/>
-      <c r="SK198" s="1"/>
-      <c r="SL198" s="1"/>
-      <c r="SM198" s="1"/>
-      <c r="SN198" s="1"/>
-      <c r="SO198" s="1"/>
-      <c r="SP198" s="1"/>
-      <c r="SQ198" s="1"/>
-      <c r="SR198" s="1"/>
-      <c r="SS198" s="1"/>
-      <c r="ST198" s="1"/>
-      <c r="SU198" s="1"/>
-      <c r="SV198" s="1"/>
-      <c r="SW198" s="1"/>
-      <c r="SX198" s="1"/>
-      <c r="SY198" s="1"/>
-      <c r="SZ198" s="1"/>
-      <c r="TA198" s="1"/>
-      <c r="TB198" s="1"/>
-      <c r="TC198" s="1"/>
-      <c r="TD198" s="1"/>
-      <c r="TE198" s="1"/>
-      <c r="TF198" s="1"/>
-      <c r="TG198" s="1"/>
-      <c r="TH198" s="1"/>
-      <c r="TI198" s="1"/>
-      <c r="TJ198" s="1"/>
-      <c r="TK198" s="1"/>
-      <c r="TL198" s="1"/>
-      <c r="TM198" s="1"/>
-      <c r="TN198" s="1"/>
-      <c r="TO198" s="1"/>
-      <c r="TP198" s="1"/>
-      <c r="TQ198" s="1"/>
-      <c r="TR198" s="1"/>
-      <c r="TS198" s="1"/>
-      <c r="TT198" s="1"/>
-      <c r="TU198" s="1"/>
-      <c r="TV198" s="1"/>
-      <c r="TW198" s="1"/>
-      <c r="TX198" s="1"/>
-      <c r="TY198" s="1"/>
-      <c r="TZ198" s="1"/>
-      <c r="UA198" s="1"/>
-      <c r="UB198" s="1"/>
-      <c r="UC198" s="1"/>
-      <c r="UD198" s="1"/>
-      <c r="UE198" s="1"/>
-      <c r="UF198" s="1"/>
-      <c r="UG198" s="1"/>
-      <c r="UH198" s="1"/>
-      <c r="UI198" s="1"/>
-      <c r="UJ198" s="1"/>
-      <c r="UK198" s="1"/>
-      <c r="UL198" s="1"/>
-      <c r="UM198" s="1"/>
-      <c r="UN198" s="1"/>
-      <c r="UO198" s="1"/>
-      <c r="UP198" s="1"/>
-      <c r="UQ198" s="1"/>
-      <c r="UR198" s="1"/>
-      <c r="US198" s="1"/>
-      <c r="UT198" s="1"/>
-      <c r="UU198" s="1"/>
-      <c r="UV198" s="1"/>
-      <c r="UW198" s="1"/>
-      <c r="UX198" s="1"/>
-      <c r="UY198" s="1"/>
-      <c r="UZ198" s="1"/>
-      <c r="VA198" s="1"/>
-      <c r="VB198" s="1"/>
-      <c r="VC198" s="1"/>
-      <c r="VD198" s="1"/>
-      <c r="VE198" s="1"/>
-      <c r="VF198" s="1"/>
-      <c r="VG198" s="1"/>
-      <c r="VH198" s="1"/>
-      <c r="VI198" s="1"/>
-      <c r="VJ198" s="1"/>
-      <c r="VK198" s="1"/>
-      <c r="VL198" s="1"/>
-      <c r="VM198" s="1"/>
-      <c r="VN198" s="1"/>
-      <c r="VO198" s="1"/>
-      <c r="VP198" s="1"/>
-      <c r="VQ198" s="1"/>
-      <c r="VR198" s="1"/>
-      <c r="VS198" s="1"/>
-      <c r="VT198" s="1"/>
-      <c r="VU198" s="1"/>
-      <c r="VV198" s="1"/>
-      <c r="VW198" s="1"/>
-      <c r="VX198" s="1"/>
-      <c r="VY198" s="1"/>
-      <c r="VZ198" s="1"/>
-      <c r="WA198" s="1"/>
-      <c r="WB198" s="1"/>
-      <c r="WC198" s="1"/>
-      <c r="WD198" s="1"/>
-      <c r="WE198" s="1"/>
-      <c r="WF198" s="1"/>
-      <c r="WG198" s="1"/>
-      <c r="WH198" s="1"/>
-      <c r="WI198" s="1"/>
-      <c r="WJ198" s="1"/>
-      <c r="WK198" s="1"/>
-      <c r="WL198" s="1"/>
-      <c r="WM198" s="1"/>
-      <c r="WN198" s="1"/>
-      <c r="WO198" s="1"/>
-      <c r="WP198" s="1"/>
-      <c r="WQ198" s="1"/>
-      <c r="WR198" s="1"/>
-      <c r="WS198" s="1"/>
-      <c r="WT198" s="1"/>
-      <c r="WU198" s="1"/>
-      <c r="WV198" s="1"/>
-      <c r="WW198" s="1"/>
-      <c r="WX198" s="1"/>
-      <c r="WY198" s="1"/>
-      <c r="WZ198" s="1"/>
-      <c r="XA198" s="1"/>
-      <c r="XB198" s="1"/>
-      <c r="XC198" s="1"/>
-      <c r="XD198" s="1"/>
-      <c r="XE198" s="1"/>
-      <c r="XF198" s="1"/>
-      <c r="XG198" s="1"/>
-      <c r="XH198" s="1"/>
-      <c r="XI198" s="1"/>
-      <c r="XJ198" s="1"/>
-      <c r="XK198" s="1"/>
-      <c r="XL198" s="1"/>
-      <c r="XM198" s="1"/>
-      <c r="XN198" s="1"/>
-      <c r="XO198" s="1"/>
-      <c r="XP198" s="1"/>
-      <c r="XQ198" s="1"/>
-      <c r="XR198" s="1"/>
-      <c r="XS198" s="1"/>
-      <c r="XT198" s="1"/>
-      <c r="XU198" s="1"/>
-      <c r="XV198" s="1"/>
-      <c r="XW198" s="1"/>
-      <c r="XX198" s="1"/>
-      <c r="XY198" s="1"/>
-      <c r="XZ198" s="1"/>
-      <c r="YA198" s="1"/>
-      <c r="YB198" s="1"/>
-      <c r="YC198" s="1"/>
-      <c r="YD198" s="1"/>
-      <c r="YE198" s="1"/>
-      <c r="YF198" s="1"/>
-      <c r="YG198" s="1"/>
-      <c r="YH198" s="1"/>
-      <c r="YI198" s="1"/>
-      <c r="YJ198" s="1"/>
-      <c r="YK198" s="1"/>
-      <c r="YL198" s="1"/>
-      <c r="YM198" s="1"/>
-      <c r="YN198" s="1"/>
-      <c r="YO198" s="1"/>
-      <c r="YP198" s="1"/>
-      <c r="YQ198" s="1"/>
-      <c r="YR198" s="1"/>
-      <c r="YS198" s="1"/>
-      <c r="YT198" s="1"/>
-      <c r="YU198" s="1"/>
-      <c r="YV198" s="1"/>
-      <c r="YW198" s="1"/>
-      <c r="YX198" s="1"/>
-      <c r="YY198" s="1"/>
-      <c r="YZ198" s="1"/>
-      <c r="ZA198" s="1"/>
-      <c r="ZB198" s="1"/>
-      <c r="ZC198" s="1"/>
-      <c r="ZD198" s="1"/>
-      <c r="ZE198" s="1"/>
-      <c r="ZF198" s="1"/>
-      <c r="ZG198" s="1"/>
-      <c r="ZH198" s="1"/>
-      <c r="ZI198" s="1"/>
-      <c r="ZJ198" s="1"/>
-      <c r="ZK198" s="1"/>
-      <c r="ZL198" s="1"/>
-      <c r="ZM198" s="1"/>
-      <c r="ZN198" s="1"/>
-      <c r="ZO198" s="1"/>
-      <c r="ZP198" s="1"/>
-      <c r="ZQ198" s="1"/>
-      <c r="ZR198" s="1"/>
-      <c r="ZS198" s="1"/>
-      <c r="ZT198" s="1"/>
-      <c r="ZU198" s="1"/>
-      <c r="ZV198" s="1"/>
-      <c r="ZW198" s="1"/>
-      <c r="ZX198" s="1"/>
-      <c r="ZY198" s="1"/>
-      <c r="ZZ198" s="1"/>
-      <c r="AAA198" s="1"/>
-      <c r="AAB198" s="1"/>
-      <c r="AAC198" s="1"/>
-      <c r="AAD198" s="1"/>
-      <c r="AAE198" s="1"/>
-      <c r="AAF198" s="1"/>
-      <c r="AAG198" s="1"/>
-      <c r="AAH198" s="1"/>
-      <c r="AAI198" s="1"/>
-      <c r="AAJ198" s="1"/>
-      <c r="AAK198" s="1"/>
-      <c r="AAL198" s="1"/>
-      <c r="AAM198" s="1"/>
-      <c r="AAN198" s="1"/>
-      <c r="AAO198" s="1"/>
-      <c r="AAP198" s="1"/>
-      <c r="AAQ198" s="1"/>
-      <c r="AAR198" s="1"/>
-      <c r="AAS198" s="1"/>
-      <c r="AAT198" s="1"/>
-      <c r="AAU198" s="1"/>
-      <c r="AAV198" s="1"/>
-      <c r="AAW198" s="1"/>
-      <c r="AAX198" s="1"/>
-      <c r="AAY198" s="1"/>
-      <c r="AAZ198" s="1"/>
-      <c r="ABA198" s="1"/>
-      <c r="ABB198" s="1"/>
-      <c r="ABC198" s="1"/>
-      <c r="ABD198" s="1"/>
-      <c r="ABE198" s="1"/>
-      <c r="ABF198" s="1"/>
-      <c r="ABG198" s="1"/>
-      <c r="ABH198" s="1"/>
-      <c r="ABI198" s="1"/>
-      <c r="ABJ198" s="1"/>
-      <c r="ABK198" s="1"/>
-      <c r="ABL198" s="1"/>
-      <c r="ABM198" s="1"/>
-      <c r="ABN198" s="1"/>
-      <c r="ABO198" s="1"/>
-      <c r="ABP198" s="1"/>
-      <c r="ABQ198" s="1"/>
-      <c r="ABR198" s="1"/>
-      <c r="ABS198" s="1"/>
-      <c r="ABT198" s="1"/>
-      <c r="ABU198" s="1"/>
-      <c r="ABV198" s="1"/>
-      <c r="ABW198" s="1"/>
-      <c r="ABX198" s="1"/>
-      <c r="ABY198" s="1"/>
-      <c r="ABZ198" s="1"/>
-      <c r="ACA198" s="1"/>
-      <c r="ACB198" s="1"/>
-      <c r="ACC198" s="1"/>
-      <c r="ACD198" s="1"/>
-      <c r="ACE198" s="1"/>
-      <c r="ACF198" s="1"/>
-      <c r="ACG198" s="1"/>
-      <c r="ACH198" s="1"/>
-      <c r="ACI198" s="1"/>
-      <c r="ACJ198" s="1"/>
-      <c r="ACK198" s="1"/>
-      <c r="ACL198" s="1"/>
-      <c r="ACM198" s="1"/>
-      <c r="ACN198" s="1"/>
-      <c r="ACO198" s="1"/>
-      <c r="ACP198" s="1"/>
-      <c r="ACQ198" s="1"/>
-      <c r="ACR198" s="1"/>
-      <c r="ACS198" s="1"/>
-      <c r="ACT198" s="1"/>
-      <c r="ACU198" s="1"/>
-      <c r="ACV198" s="1"/>
-      <c r="ACW198" s="1"/>
-      <c r="ACX198" s="1"/>
-      <c r="ACY198" s="1"/>
-      <c r="ACZ198" s="1"/>
-      <c r="ADA198" s="1"/>
-      <c r="ADB198" s="1"/>
-      <c r="ADC198" s="1"/>
-      <c r="ADD198" s="1"/>
-      <c r="ADE198" s="1"/>
-      <c r="ADF198" s="1"/>
-      <c r="ADG198" s="1"/>
-      <c r="ADH198" s="1"/>
-      <c r="ADI198" s="1"/>
-      <c r="ADJ198" s="1"/>
-      <c r="ADK198" s="1"/>
-      <c r="ADL198" s="1"/>
-      <c r="ADM198" s="1"/>
-      <c r="ADN198" s="1"/>
-      <c r="ADO198" s="1"/>
-      <c r="ADP198" s="1"/>
-      <c r="ADQ198" s="1"/>
-      <c r="ADR198" s="1"/>
-      <c r="ADS198" s="1"/>
-      <c r="ADT198" s="1"/>
-      <c r="ADU198" s="1"/>
-      <c r="ADV198" s="1"/>
-      <c r="ADW198" s="1"/>
-      <c r="ADX198" s="1"/>
-      <c r="ADY198" s="1"/>
-      <c r="ADZ198" s="1"/>
-      <c r="AEA198" s="1"/>
-      <c r="AEB198" s="1"/>
-      <c r="AEC198" s="1"/>
-      <c r="AED198" s="1"/>
-      <c r="AEE198" s="1"/>
-      <c r="AEF198" s="1"/>
-      <c r="AEG198" s="1"/>
-      <c r="AEH198" s="1"/>
-      <c r="AEI198" s="1"/>
-      <c r="AEJ198" s="1"/>
-      <c r="AEK198" s="1"/>
-      <c r="AEL198" s="1"/>
-      <c r="AEM198" s="1"/>
-      <c r="AEN198" s="1"/>
-      <c r="AEO198" s="1"/>
-      <c r="AEP198" s="1"/>
-      <c r="AEQ198" s="1"/>
-      <c r="AER198" s="1"/>
-      <c r="AES198" s="1"/>
-      <c r="AET198" s="1"/>
-      <c r="AEU198" s="1"/>
-      <c r="AEV198" s="1"/>
-      <c r="AEW198" s="1"/>
-      <c r="AEX198" s="1"/>
-      <c r="AEY198" s="1"/>
-      <c r="AEZ198" s="1"/>
-      <c r="AFA198" s="1"/>
-      <c r="AFB198" s="1"/>
-      <c r="AFC198" s="1"/>
-      <c r="AFD198" s="1"/>
-      <c r="AFE198" s="1"/>
-      <c r="AFF198" s="1"/>
-      <c r="AFG198" s="1"/>
-      <c r="AFH198" s="1"/>
-      <c r="AFI198" s="1"/>
-      <c r="AFJ198" s="1"/>
-      <c r="AFK198" s="1"/>
-      <c r="AFL198" s="1"/>
-      <c r="AFM198" s="1"/>
-      <c r="AFN198" s="1"/>
-      <c r="AFO198" s="1"/>
-      <c r="AFP198" s="1"/>
-      <c r="AFQ198" s="1"/>
-      <c r="AFR198" s="1"/>
-      <c r="AFS198" s="1"/>
-      <c r="AFT198" s="1"/>
-      <c r="AFU198" s="1"/>
-      <c r="AFV198" s="1"/>
-      <c r="AFW198" s="1"/>
-      <c r="AFX198" s="1"/>
-      <c r="AFY198" s="1"/>
-      <c r="AFZ198" s="1"/>
-      <c r="AGA198" s="1"/>
-      <c r="AGB198" s="1"/>
-      <c r="AGC198" s="1"/>
-      <c r="AGD198" s="1"/>
-      <c r="AGE198" s="1"/>
-      <c r="AGF198" s="1"/>
-      <c r="AGG198" s="1"/>
-      <c r="AGH198" s="1"/>
-      <c r="AGI198" s="1"/>
-      <c r="AGJ198" s="1"/>
-      <c r="AGK198" s="1"/>
-      <c r="AGL198" s="1"/>
-      <c r="AGM198" s="1"/>
-      <c r="AGN198" s="1"/>
-      <c r="AGO198" s="1"/>
-      <c r="AGP198" s="1"/>
-      <c r="AGQ198" s="1"/>
-      <c r="AGR198" s="1"/>
-      <c r="AGS198" s="1"/>
-      <c r="AGT198" s="1"/>
-      <c r="AGU198" s="1"/>
-      <c r="AGV198" s="1"/>
-      <c r="AGW198" s="1"/>
-      <c r="AGX198" s="1"/>
-      <c r="AGY198" s="1"/>
-      <c r="AGZ198" s="1"/>
-      <c r="AHA198" s="1"/>
-      <c r="AHB198" s="1"/>
-      <c r="AHC198" s="1"/>
-      <c r="AHD198" s="1"/>
-      <c r="AHE198" s="1"/>
-      <c r="AHF198" s="1"/>
-      <c r="AHG198" s="1"/>
-      <c r="AHH198" s="1"/>
-      <c r="AHI198" s="1"/>
-      <c r="AHJ198" s="1"/>
-      <c r="AHK198" s="1"/>
-      <c r="AHL198" s="1"/>
-      <c r="AHM198" s="1"/>
-      <c r="AHN198" s="1"/>
-      <c r="AHO198" s="1"/>
-      <c r="AHP198" s="1"/>
-      <c r="AHQ198" s="1"/>
-      <c r="AHR198" s="1"/>
-      <c r="AHS198" s="1"/>
-      <c r="AHT198" s="1"/>
-      <c r="AHU198" s="1"/>
-      <c r="AHV198" s="1"/>
-      <c r="AHW198" s="1"/>
-      <c r="AHX198" s="1"/>
-      <c r="AHY198" s="1"/>
-      <c r="AHZ198" s="1"/>
-      <c r="AIA198" s="1"/>
-      <c r="AIB198" s="1"/>
-      <c r="AIC198" s="1"/>
-      <c r="AID198" s="1"/>
-      <c r="AIE198" s="1"/>
-      <c r="AIF198" s="1"/>
-      <c r="AIG198" s="1"/>
-      <c r="AIH198" s="1"/>
-      <c r="AII198" s="1"/>
-      <c r="AIJ198" s="1"/>
-      <c r="AIK198" s="1"/>
-      <c r="AIL198" s="1"/>
-      <c r="AIM198" s="1"/>
-      <c r="AIN198" s="1"/>
-      <c r="AIO198" s="1"/>
-      <c r="AIP198" s="1"/>
-      <c r="AIQ198" s="1"/>
-      <c r="AIR198" s="1"/>
-      <c r="AIS198" s="1"/>
-      <c r="AIT198" s="1"/>
-      <c r="AIU198" s="1"/>
-      <c r="AIV198" s="1"/>
-      <c r="AIW198" s="1"/>
-      <c r="AIX198" s="1"/>
-      <c r="AIY198" s="1"/>
-      <c r="AIZ198" s="1"/>
-      <c r="AJA198" s="1"/>
-      <c r="AJB198" s="1"/>
-      <c r="AJC198" s="1"/>
-      <c r="AJD198" s="1"/>
-      <c r="AJE198" s="1"/>
-      <c r="AJF198" s="1"/>
-      <c r="AJG198" s="1"/>
-      <c r="AJH198" s="1"/>
-      <c r="AJI198" s="1"/>
-      <c r="AJJ198" s="1"/>
-      <c r="AJK198" s="1"/>
-      <c r="AJL198" s="1"/>
-      <c r="AJM198" s="1"/>
-      <c r="AJN198" s="1"/>
-      <c r="AJO198" s="1"/>
-      <c r="AJP198" s="1"/>
-      <c r="AJQ198" s="1"/>
-      <c r="AJR198" s="1"/>
-      <c r="AJS198" s="1"/>
-      <c r="AJT198" s="1"/>
-      <c r="AJU198" s="1"/>
-      <c r="AJV198" s="1"/>
-      <c r="AJW198" s="1"/>
-      <c r="AJX198" s="1"/>
-      <c r="AJY198" s="1"/>
-      <c r="AJZ198" s="1"/>
-      <c r="AKA198" s="1"/>
-      <c r="AKB198" s="1"/>
-      <c r="AKC198" s="1"/>
-      <c r="AKD198" s="1"/>
-      <c r="AKE198" s="1"/>
-      <c r="AKF198" s="1"/>
-      <c r="AKG198" s="1"/>
-      <c r="AKH198" s="1"/>
-      <c r="AKI198" s="1"/>
-      <c r="AKJ198" s="1"/>
-      <c r="AKK198" s="1"/>
-      <c r="AKL198" s="1"/>
-      <c r="AKM198" s="1"/>
-      <c r="AKN198" s="1"/>
-      <c r="AKO198" s="1"/>
-      <c r="AKP198" s="1"/>
-      <c r="AKQ198" s="1"/>
-      <c r="AKR198" s="1"/>
-      <c r="AKS198" s="1"/>
-      <c r="AKT198" s="1"/>
-      <c r="AKU198" s="1"/>
-      <c r="AKV198" s="1"/>
-      <c r="AKW198" s="1"/>
-      <c r="AKX198" s="1"/>
-      <c r="AKY198" s="1"/>
-      <c r="AKZ198" s="1"/>
-      <c r="ALA198" s="1"/>
-      <c r="ALB198" s="1"/>
-      <c r="ALC198" s="1"/>
-      <c r="ALD198" s="1"/>
-      <c r="ALE198" s="1"/>
-      <c r="ALF198" s="1"/>
-      <c r="ALG198" s="1"/>
-      <c r="ALH198" s="1"/>
-      <c r="ALI198" s="1"/>
-      <c r="ALJ198" s="1"/>
-      <c r="ALK198" s="1"/>
-      <c r="ALL198" s="1"/>
-      <c r="ALM198" s="1"/>
-      <c r="ALN198" s="1"/>
-      <c r="ALO198" s="1"/>
-      <c r="ALP198" s="1"/>
-      <c r="ALQ198" s="1"/>
-      <c r="ALR198" s="1"/>
-      <c r="ALS198" s="1"/>
-      <c r="ALT198" s="1"/>
-      <c r="ALU198" s="1"/>
-      <c r="ALV198" s="1"/>
-      <c r="ALW198" s="1"/>
-      <c r="ALX198" s="1"/>
-      <c r="ALY198" s="1"/>
-      <c r="ALZ198" s="1"/>
-      <c r="AMA198" s="1"/>
-      <c r="AMB198" s="1"/>
-      <c r="AMC198" s="1"/>
-      <c r="AMD198" s="1"/>
-      <c r="AME198" s="1"/>
-      <c r="AMF198" s="1"/>
-      <c r="AMG198" s="1"/>
-      <c r="AMH198" s="1"/>
-      <c r="AMI198" s="1"/>
-      <c r="AMJ198" s="1"/>
     </row>
     <row r="199" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="15"/>
@@ -5353,6 +5383,7 @@
       <c r="C201" s="35"/>
       <c r="D201" s="38"/>
       <c r="E201" s="36"/>
+      <c r="F201" s="36"/>
       <c r="G201" s="36"/>
       <c r="H201" s="36"/>
       <c r="I201" s="36"/>
@@ -5369,17 +5400,9 @@
       <c r="B202" s="35"/>
       <c r="C202" s="35"/>
       <c r="D202" s="38"/>
-      <c r="E202" s="36"/>
-      <c r="G202" s="36"/>
-      <c r="H202" s="36"/>
-      <c r="I202" s="36"/>
-      <c r="J202" s="37"/>
-      <c r="K202" s="37"/>
-      <c r="L202" s="35"/>
       <c r="M202" s="35"/>
       <c r="N202" s="35"/>
       <c r="O202" s="38"/>
-      <c r="P202" s="36"/>
       <c r="Q202" s="5"/>
       <c r="R202" s="5"/>
       <c r="S202" s="5"/>
@@ -6390,68 +6413,98 @@
       <c r="AMJ202" s="5"/>
     </row>
     <row r="203" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B203" s="35"/>
-      <c r="C203" s="35"/>
-      <c r="D203" s="38"/>
-      <c r="E203" s="36"/>
-      <c r="G203" s="36"/>
-      <c r="H203" s="36"/>
-      <c r="I203" s="36"/>
-      <c r="J203" s="37"/>
-      <c r="K203" s="37"/>
-      <c r="L203" s="35"/>
-      <c r="M203" s="35"/>
-      <c r="N203" s="35"/>
-      <c r="O203" s="38"/>
-      <c r="P203" s="36"/>
+      <c r="B203" s="5"/>
+      <c r="C203" s="5"/>
+      <c r="D203" s="5"/>
+      <c r="E203" s="5"/>
+      <c r="F203" s="5"/>
+      <c r="G203" s="5"/>
+      <c r="H203" s="5"/>
+      <c r="I203" s="5"/>
+      <c r="J203" s="5"/>
+      <c r="K203" s="5"/>
+      <c r="L203" s="5"/>
+      <c r="M203" s="5"/>
+      <c r="N203" s="5"/>
+      <c r="O203" s="5"/>
+      <c r="P203" s="5"/>
     </row>
     <row r="204" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="26"/>
-      <c r="B204" s="35"/>
-      <c r="C204" s="35"/>
-      <c r="D204" s="38"/>
-      <c r="E204" s="36"/>
-      <c r="G204" s="36"/>
-      <c r="H204" s="36"/>
-      <c r="I204" s="36"/>
-      <c r="J204" s="37"/>
-      <c r="K204" s="37"/>
-      <c r="L204" s="35"/>
-      <c r="M204" s="35"/>
-      <c r="N204" s="35"/>
-      <c r="O204" s="38"/>
-      <c r="P204" s="36"/>
+      <c r="B204" s="5"/>
+      <c r="C204" s="5"/>
+      <c r="D204" s="5"/>
+      <c r="E204" s="5"/>
+      <c r="F204" s="5"/>
+      <c r="G204" s="5"/>
+      <c r="H204" s="5"/>
+      <c r="I204" s="5"/>
+      <c r="J204" s="5"/>
+      <c r="K204" s="5"/>
+      <c r="L204" s="5"/>
+      <c r="M204" s="5"/>
+      <c r="N204" s="5"/>
+      <c r="O204" s="5"/>
+      <c r="P204" s="5"/>
     </row>
     <row r="205" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="26"/>
-      <c r="B205" s="35"/>
-      <c r="C205" s="35"/>
-      <c r="D205" s="38"/>
-      <c r="E205" s="36"/>
-      <c r="F205" s="36"/>
-      <c r="G205" s="36"/>
-      <c r="H205" s="36"/>
-      <c r="I205" s="36"/>
-      <c r="J205" s="37"/>
-      <c r="K205" s="37"/>
-      <c r="L205" s="35"/>
-      <c r="M205" s="35"/>
-      <c r="N205" s="35"/>
-      <c r="O205" s="38"/>
-      <c r="P205" s="36"/>
+      <c r="B205" s="5"/>
+      <c r="C205" s="5"/>
+      <c r="D205" s="5"/>
+      <c r="E205" s="5"/>
+      <c r="F205" s="5"/>
+      <c r="G205" s="5"/>
+      <c r="H205" s="5"/>
+      <c r="I205" s="5"/>
+      <c r="J205" s="5"/>
+      <c r="K205" s="5"/>
+      <c r="L205" s="5"/>
+      <c r="M205" s="5"/>
+      <c r="N205" s="5"/>
+      <c r="O205" s="5"/>
+      <c r="P205" s="5"/>
     </row>
     <row r="206" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N206" s="41"/>
+      <c r="B206" s="5"/>
+      <c r="C206" s="5"/>
+      <c r="D206" s="5"/>
+      <c r="E206" s="5"/>
+      <c r="F206" s="5"/>
+      <c r="G206" s="5"/>
+      <c r="H206" s="5"/>
+      <c r="I206" s="5"/>
+      <c r="J206" s="5"/>
+      <c r="K206" s="5"/>
+      <c r="L206" s="5"/>
+      <c r="M206" s="5"/>
+      <c r="N206" s="5"/>
+      <c r="O206" s="5"/>
+      <c r="P206" s="5"/>
     </row>
     <row r="207" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N207" s="41"/>
+      <c r="B207" s="5"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="5"/>
+      <c r="E207" s="5"/>
+      <c r="F207" s="5"/>
+      <c r="G207" s="5"/>
+      <c r="H207" s="5"/>
+      <c r="I207" s="5"/>
+      <c r="J207" s="5"/>
+      <c r="K207" s="5"/>
+      <c r="L207" s="5"/>
+      <c r="M207" s="5"/>
+      <c r="N207" s="5"/>
+      <c r="O207" s="5"/>
+      <c r="P207" s="5"/>
     </row>
     <row r="208" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B208" s="16" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C208" s="17" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D208" s="16"/>
       <c r="E208" s="17"/>
@@ -6488,23 +6541,23 @@
       <c r="Q210" s="5"/>
     </row>
     <row r="211" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B211" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C211" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="D211" s="42"/>
-      <c r="E211" s="43"/>
-      <c r="F211" s="43"/>
-      <c r="G211" s="43"/>
-      <c r="H211" s="43"/>
-      <c r="I211" s="43"/>
-      <c r="J211" s="43"/>
-      <c r="K211" s="43"/>
-      <c r="L211" s="43"/>
-      <c r="M211" s="43"/>
-      <c r="N211" s="43"/>
+      <c r="B211" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C211" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D211" s="41"/>
+      <c r="E211" s="42"/>
+      <c r="F211" s="42"/>
+      <c r="G211" s="42"/>
+      <c r="H211" s="42"/>
+      <c r="I211" s="42"/>
+      <c r="J211" s="42"/>
+      <c r="K211" s="42"/>
+      <c r="L211" s="42"/>
+      <c r="M211" s="42"/>
+      <c r="N211" s="42"/>
       <c r="O211" s="31"/>
       <c r="P211" s="31"/>
       <c r="Q211" s="5"/>
@@ -6521,7 +6574,7 @@
       <c r="C213" s="34"/>
       <c r="D213" s="27"/>
       <c r="E213" s="2"/>
-      <c r="O213" s="44"/>
+      <c r="O213" s="43"/>
       <c r="P213" s="27"/>
       <c r="Q213" s="27"/>
     </row>
@@ -6539,7 +6592,7 @@
       <c r="L214" s="27"/>
       <c r="M214" s="27"/>
       <c r="N214" s="27"/>
-      <c r="O214" s="44"/>
+      <c r="O214" s="43"/>
       <c r="P214" s="27"/>
       <c r="Q214" s="27"/>
     </row>
@@ -6548,7 +6601,7 @@
       <c r="C215" s="2"/>
       <c r="D215" s="1"/>
       <c r="E215" s="2"/>
-      <c r="O215" s="41"/>
+      <c r="O215" s="44"/>
     </row>
     <row r="221" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="35"/>
@@ -6646,7 +6699,7 @@
     <mergeCell ref="F1:P6"/>
   </mergeCells>
   <dataValidations count="35">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J1:J37 J118:J123 J129:J144 J148:J155 J162:K192 J193 J206:J211 K214:K215 J216:J220 J227:J1202" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J1:J37 J118:J123 J129:J144 J148:J155 J158:K159 J162:K192 J193 J208:J211 K214:K215 J216:J220 J227:J1202" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6774,15 +6827,15 @@
       <formula1>"rx,tx"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="The Object code value shall be:&#10;VARIABLE&#10;RECORD&#10;ARRAY" errorStyle="stop" errorTitle="Object Code value" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C156:C161 N156:N161 C194:C205 N194:N205 C221:C226" type="list">
+    <dataValidation allowBlank="true" error="The Object code value shall be:&#10;VARIABLE&#10;RECORD&#10;ARRAY" errorStyle="stop" errorTitle="Object Code value" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C156:C157 N156:N157 C194:C202 N194:N202 C221:C226" type="list">
       <formula1>"VARIABLE,ARRAY,RECORD"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="The value for the entry category shall be &#10;M : (mandatory)&#10;O : (optional) &#10;C : (conditional)" errorStyle="stop" errorTitle="Category" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J156 J195:J199 J201:J205 J222:J226" type="list">
+    <dataValidation allowBlank="true" error="The value for the entry category shall be &#10;M : (mandatory)&#10;O : (optional) &#10;C : (conditional)" errorStyle="stop" errorTitle="Category" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J156 J195 J197 J199 J201 J222:J226" type="list">
       <formula1>"M,O,C"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="The entry flag shall be&#10;B : (Backup)&#10;S : (Setting)" errorStyle="stop" errorTitle="Backup/Setting Flag" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K156 K195:K199 K201:K205 K222:K226" type="list">
+    <dataValidation allowBlank="true" error="The entry flag shall be&#10;B : (Backup)&#10;S : (Setting)" errorStyle="stop" errorTitle="Backup/Setting Flag" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K156 K195 K197 K199 K201 K222:K226" type="list">
       <formula1>"B,S"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>